<commit_message>
chg: updated tgt list
</commit_message>
<xml_diff>
--- a/OPAR/WORKSPACE/OPAR_JOINT_TARGET_LIST.xlsx
+++ b/OPAR/WORKSPACE/OPAR_JOINT_TARGET_LIST.xlsx
@@ -2848,9 +2848,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2936,6 +2933,63 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2975,61 +3029,19 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3038,21 +3050,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3070,6 +3067,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3109,7 +3109,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3154,7 +3154,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3204,7 +3204,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3249,7 +3249,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3299,7 +3299,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3344,7 +3344,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3394,7 +3394,7 @@
         <xdr:cNvPr id="4" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3447,7 +3447,7 @@
         <xdr:cNvPr id="3" name="TekstSylinder 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3539,7 +3539,7 @@
         <xdr:cNvPr id="2049" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3597,7 +3597,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3650,7 +3650,7 @@
         <xdr:cNvPr id="2049" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3703,7 +3703,7 @@
         <xdr:cNvPr id="4" name="TekstSylinder 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3801,7 +3801,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3854,7 +3854,7 @@
         <xdr:cNvPr id="4" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3907,7 +3907,7 @@
         <xdr:cNvPr id="5" name="TekstSylinder 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4001,7 +4001,7 @@
         <xdr:cNvPr id="5" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4054,7 +4054,7 @@
         <xdr:cNvPr id="6" name="TekstSylinder 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4149,7 +4149,7 @@
         <xdr:cNvPr id="4" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4207,7 +4207,7 @@
         <xdr:cNvPr id="3073" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000010C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000010C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4260,7 +4260,7 @@
         <xdr:cNvPr id="3074" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000020C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000020C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4313,7 +4313,7 @@
         <xdr:cNvPr id="3075" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000030C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000030C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4366,7 +4366,7 @@
         <xdr:cNvPr id="3076" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000040C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000040C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4419,7 +4419,7 @@
         <xdr:cNvPr id="3077" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000050C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000050C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4472,7 +4472,7 @@
         <xdr:cNvPr id="3078" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000060C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000060C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4525,7 +4525,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4852,7 +4852,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4868,16 +4868,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.9" customHeight="1" thickBot="1">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="94" t="s">
         <v>594</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="67"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="141"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
       <c r="A2" s="46" t="s">
@@ -4889,7 +4889,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="41"/>
-      <c r="H2" s="92"/>
+      <c r="H2" s="91"/>
     </row>
     <row r="3" spans="1:8" ht="29.45" customHeight="1" thickBot="1">
       <c r="A3" s="5" t="s">
@@ -4898,10 +4898,10 @@
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="69" t="s">
         <v>215</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -4910,7 +4910,7 @@
       <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="83" t="s">
+      <c r="G3" s="82" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -4918,16 +4918,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="71" t="s">
         <v>552</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="72" t="s">
         <v>360</v>
       </c>
-      <c r="D4" s="74"/>
+      <c r="D4" s="73"/>
       <c r="E4" s="26" t="s">
         <v>554</v>
       </c>
@@ -4942,31 +4942,31 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="83" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>553</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="84" t="s">
         <v>360</v>
       </c>
-      <c r="D5" s="86"/>
-      <c r="E5" s="87" t="s">
+      <c r="D5" s="85"/>
+      <c r="E5" s="86" t="s">
         <v>557</v>
       </c>
-      <c r="F5" s="87" t="s">
+      <c r="F5" s="86" t="s">
         <v>558</v>
       </c>
-      <c r="G5" s="86" t="s">
+      <c r="G5" s="85" t="s">
         <v>556</v>
       </c>
-      <c r="H5" s="88" t="s">
+      <c r="H5" s="87" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="67" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="26" t="s">
@@ -4990,26 +4990,26 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="87" t="s">
+      <c r="B7" s="86" t="s">
         <v>574</v>
       </c>
-      <c r="C7" s="85" t="s">
+      <c r="C7" s="84" t="s">
         <v>360</v>
       </c>
-      <c r="D7" s="86"/>
-      <c r="E7" s="87" t="s">
+      <c r="D7" s="85"/>
+      <c r="E7" s="86" t="s">
         <v>575</v>
       </c>
-      <c r="F7" s="87" t="s">
+      <c r="F7" s="86" t="s">
         <v>576</v>
       </c>
-      <c r="G7" s="86" t="s">
+      <c r="G7" s="85" t="s">
         <v>577</v>
       </c>
-      <c r="H7" s="88" t="s">
+      <c r="H7" s="87" t="s">
         <v>578</v>
       </c>
     </row>
@@ -5038,26 +5038,26 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="87" t="s">
+      <c r="B9" s="86" t="s">
         <v>542</v>
       </c>
-      <c r="C9" s="85" t="s">
+      <c r="C9" s="84" t="s">
         <v>648</v>
       </c>
-      <c r="D9" s="86"/>
-      <c r="E9" s="87" t="s">
+      <c r="D9" s="85"/>
+      <c r="E9" s="86" t="s">
         <v>543</v>
       </c>
-      <c r="F9" s="87" t="s">
+      <c r="F9" s="86" t="s">
         <v>544</v>
       </c>
-      <c r="G9" s="86" t="s">
+      <c r="G9" s="85" t="s">
         <v>545</v>
       </c>
-      <c r="H9" s="88" t="s">
+      <c r="H9" s="87" t="s">
         <v>546</v>
       </c>
     </row>
@@ -5086,26 +5086,26 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="85">
+      <c r="C11" s="84">
         <v>9</v>
       </c>
-      <c r="D11" s="86"/>
-      <c r="E11" s="87" t="s">
+      <c r="D11" s="85"/>
+      <c r="E11" s="86" t="s">
         <v>375</v>
       </c>
-      <c r="F11" s="87" t="s">
+      <c r="F11" s="86" t="s">
         <v>376</v>
       </c>
-      <c r="G11" s="86" t="s">
+      <c r="G11" s="85" t="s">
         <v>390</v>
       </c>
-      <c r="H11" s="88" t="s">
+      <c r="H11" s="87" t="s">
         <v>598</v>
       </c>
     </row>
@@ -5134,26 +5134,26 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="C13" s="85">
+      <c r="C13" s="84">
         <v>9</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="87" t="s">
+      <c r="D13" s="85"/>
+      <c r="E13" s="86" t="s">
         <v>358</v>
       </c>
-      <c r="F13" s="87" t="s">
+      <c r="F13" s="86" t="s">
         <v>359</v>
       </c>
-      <c r="G13" s="86">
+      <c r="G13" s="85">
         <v>1654</v>
       </c>
-      <c r="H13" s="88" t="s">
+      <c r="H13" s="87" t="s">
         <v>603</v>
       </c>
     </row>
@@ -5182,26 +5182,26 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="87" t="s">
+      <c r="B15" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="85">
+      <c r="C15" s="84">
         <v>9</v>
       </c>
-      <c r="D15" s="86"/>
-      <c r="E15" s="87" t="s">
+      <c r="D15" s="85"/>
+      <c r="E15" s="86" t="s">
         <v>404</v>
       </c>
-      <c r="F15" s="87" t="s">
+      <c r="F15" s="86" t="s">
         <v>405</v>
       </c>
-      <c r="G15" s="86">
+      <c r="G15" s="85">
         <v>1152</v>
       </c>
-      <c r="H15" s="88" t="s">
+      <c r="H15" s="87" t="s">
         <v>610</v>
       </c>
     </row>
@@ -5230,26 +5230,26 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="85">
+      <c r="C17" s="84">
         <v>9</v>
       </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="87" t="s">
+      <c r="D17" s="85"/>
+      <c r="E17" s="86" t="s">
         <v>397</v>
       </c>
-      <c r="F17" s="87" t="s">
+      <c r="F17" s="86" t="s">
         <v>398</v>
       </c>
-      <c r="G17" s="86">
+      <c r="G17" s="85">
         <v>2096</v>
       </c>
-      <c r="H17" s="88" t="s">
+      <c r="H17" s="87" t="s">
         <v>634</v>
       </c>
     </row>
@@ -5278,26 +5278,26 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="89" t="s">
+      <c r="A19" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="87" t="s">
+      <c r="B19" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="85">
+      <c r="C19" s="84">
         <v>9</v>
       </c>
-      <c r="D19" s="86"/>
-      <c r="E19" s="87" t="s">
+      <c r="D19" s="85"/>
+      <c r="E19" s="86" t="s">
         <v>331</v>
       </c>
-      <c r="F19" s="87" t="s">
+      <c r="F19" s="86" t="s">
         <v>332</v>
       </c>
-      <c r="G19" s="86" t="s">
+      <c r="G19" s="85" t="s">
         <v>333</v>
       </c>
-      <c r="H19" s="88" t="s">
+      <c r="H19" s="87" t="s">
         <v>602</v>
       </c>
     </row>
@@ -5326,31 +5326,31 @@
       </c>
     </row>
     <row r="21" spans="1:8" s="50" customFormat="1">
-      <c r="A21" s="84" t="s">
+      <c r="A21" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="87" t="s">
+      <c r="B21" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="C21" s="85">
+      <c r="C21" s="84">
         <v>9</v>
       </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="87" t="s">
+      <c r="D21" s="85"/>
+      <c r="E21" s="86" t="s">
         <v>352</v>
       </c>
-      <c r="F21" s="87" t="s">
+      <c r="F21" s="86" t="s">
         <v>353</v>
       </c>
-      <c r="G21" s="86" t="s">
+      <c r="G21" s="85" t="s">
         <v>354</v>
       </c>
-      <c r="H21" s="88" t="s">
+      <c r="H21" s="87" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30">
-      <c r="A22" s="68" t="s">
+      <c r="A22" s="67" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="26" t="s">
@@ -5374,31 +5374,31 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="30">
-      <c r="A23" s="84" t="s">
+      <c r="A23" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="86" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="85">
+      <c r="C23" s="84">
         <v>9</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="87" t="s">
+      <c r="D23" s="85"/>
+      <c r="E23" s="86" t="s">
         <v>533</v>
       </c>
-      <c r="F23" s="87" t="s">
+      <c r="F23" s="86" t="s">
         <v>534</v>
       </c>
-      <c r="G23" s="86" t="s">
+      <c r="G23" s="85" t="s">
         <v>535</v>
       </c>
-      <c r="H23" s="88" t="s">
+      <c r="H23" s="87" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="68" t="s">
+      <c r="A24" s="67" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="26" t="s">
@@ -5422,31 +5422,31 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="30">
-      <c r="A25" s="84" t="s">
+      <c r="A25" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="85" t="s">
+      <c r="C25" s="84" t="s">
         <v>275</v>
       </c>
-      <c r="D25" s="86"/>
-      <c r="E25" s="87" t="s">
+      <c r="D25" s="85"/>
+      <c r="E25" s="86" t="s">
         <v>369</v>
       </c>
-      <c r="F25" s="87" t="s">
+      <c r="F25" s="86" t="s">
         <v>370</v>
       </c>
-      <c r="G25" s="86" t="s">
+      <c r="G25" s="85" t="s">
         <v>371</v>
       </c>
-      <c r="H25" s="88" t="s">
+      <c r="H25" s="87" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30">
-      <c r="A26" s="68" t="s">
+      <c r="A26" s="67" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="26" t="s">
@@ -5470,26 +5470,26 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="30">
-      <c r="A27" s="89" t="s">
+      <c r="A27" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="87" t="s">
+      <c r="B27" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="C27" s="85">
+      <c r="C27" s="84">
         <v>9</v>
       </c>
-      <c r="D27" s="86"/>
-      <c r="E27" s="87" t="s">
+      <c r="D27" s="85"/>
+      <c r="E27" s="86" t="s">
         <v>501</v>
       </c>
-      <c r="F27" s="87" t="s">
+      <c r="F27" s="86" t="s">
         <v>502</v>
       </c>
-      <c r="G27" s="86" t="s">
+      <c r="G27" s="85" t="s">
         <v>503</v>
       </c>
-      <c r="H27" s="88" t="s">
+      <c r="H27" s="87" t="s">
         <v>504</v>
       </c>
     </row>
@@ -5518,26 +5518,26 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="89" t="s">
+      <c r="A29" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="87" t="s">
+      <c r="B29" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="C29" s="85">
+      <c r="C29" s="84">
         <v>9</v>
       </c>
-      <c r="D29" s="86"/>
-      <c r="E29" s="87" t="s">
+      <c r="D29" s="85"/>
+      <c r="E29" s="86" t="s">
         <v>497</v>
       </c>
-      <c r="F29" s="87" t="s">
+      <c r="F29" s="86" t="s">
         <v>498</v>
       </c>
-      <c r="G29" s="86" t="s">
+      <c r="G29" s="85" t="s">
         <v>499</v>
       </c>
-      <c r="H29" s="88" t="s">
+      <c r="H29" s="87" t="s">
         <v>500</v>
       </c>
     </row>
@@ -5566,26 +5566,26 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="89" t="s">
+      <c r="A31" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="87" t="s">
+      <c r="B31" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="85">
+      <c r="C31" s="84">
         <v>9</v>
       </c>
-      <c r="D31" s="86"/>
-      <c r="E31" s="87" t="s">
+      <c r="D31" s="85"/>
+      <c r="E31" s="86" t="s">
         <v>523</v>
       </c>
-      <c r="F31" s="87" t="s">
+      <c r="F31" s="86" t="s">
         <v>524</v>
       </c>
-      <c r="G31" s="86" t="s">
+      <c r="G31" s="85" t="s">
         <v>525</v>
       </c>
-      <c r="H31" s="88" t="s">
+      <c r="H31" s="87" t="s">
         <v>529</v>
       </c>
     </row>
@@ -5599,7 +5599,7 @@
       <c r="C32" s="64">
         <v>9</v>
       </c>
-      <c r="D32" s="80"/>
+      <c r="D32" s="79"/>
       <c r="E32" s="26" t="s">
         <v>526</v>
       </c>
@@ -5614,26 +5614,26 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="89" t="s">
+      <c r="A33" s="88" t="s">
         <v>112</v>
       </c>
-      <c r="B33" s="87" t="s">
+      <c r="B33" s="86" t="s">
         <v>183</v>
       </c>
-      <c r="C33" s="85">
+      <c r="C33" s="84">
         <v>9</v>
       </c>
-      <c r="D33" s="90"/>
-      <c r="E33" s="87" t="s">
+      <c r="D33" s="89"/>
+      <c r="E33" s="86" t="s">
         <v>493</v>
       </c>
-      <c r="F33" s="87" t="s">
+      <c r="F33" s="86" t="s">
         <v>494</v>
       </c>
-      <c r="G33" s="86" t="s">
+      <c r="G33" s="85" t="s">
         <v>495</v>
       </c>
-      <c r="H33" s="88" t="s">
+      <c r="H33" s="87" t="s">
         <v>496</v>
       </c>
     </row>
@@ -5647,7 +5647,7 @@
       <c r="C34" s="64">
         <v>9</v>
       </c>
-      <c r="D34" s="80"/>
+      <c r="D34" s="79"/>
       <c r="E34" s="26" t="s">
         <v>505</v>
       </c>
@@ -5662,26 +5662,26 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="30">
-      <c r="A35" s="89" t="s">
+      <c r="A35" s="88" t="s">
         <v>114</v>
       </c>
-      <c r="B35" s="87" t="s">
+      <c r="B35" s="86" t="s">
         <v>183</v>
       </c>
-      <c r="C35" s="85">
+      <c r="C35" s="84">
         <v>9</v>
       </c>
-      <c r="D35" s="90"/>
-      <c r="E35" s="87" t="s">
+      <c r="D35" s="89"/>
+      <c r="E35" s="86" t="s">
         <v>509</v>
       </c>
-      <c r="F35" s="87" t="s">
+      <c r="F35" s="86" t="s">
         <v>510</v>
       </c>
-      <c r="G35" s="86" t="s">
+      <c r="G35" s="85" t="s">
         <v>503</v>
       </c>
-      <c r="H35" s="88" t="s">
+      <c r="H35" s="87" t="s">
         <v>511</v>
       </c>
     </row>
@@ -5695,7 +5695,7 @@
       <c r="C36" s="64">
         <v>9</v>
       </c>
-      <c r="D36" s="80"/>
+      <c r="D36" s="79"/>
       <c r="E36" s="26" t="s">
         <v>516</v>
       </c>
@@ -5710,26 +5710,26 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="45">
-      <c r="A37" s="89" t="s">
+      <c r="A37" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="B37" s="87" t="s">
+      <c r="B37" s="86" t="s">
         <v>184</v>
       </c>
-      <c r="C37" s="85" t="s">
+      <c r="C37" s="84" t="s">
         <v>272</v>
       </c>
-      <c r="D37" s="90"/>
-      <c r="E37" s="87" t="s">
+      <c r="D37" s="89"/>
+      <c r="E37" s="86" t="s">
         <v>482</v>
       </c>
-      <c r="F37" s="87" t="s">
+      <c r="F37" s="86" t="s">
         <v>483</v>
       </c>
-      <c r="G37" s="86" t="s">
+      <c r="G37" s="85" t="s">
         <v>484</v>
       </c>
-      <c r="H37" s="88" t="s">
+      <c r="H37" s="87" t="s">
         <v>485</v>
       </c>
     </row>
@@ -5743,7 +5743,7 @@
       <c r="C38" s="64" t="s">
         <v>272</v>
       </c>
-      <c r="D38" s="80"/>
+      <c r="D38" s="79"/>
       <c r="E38" s="26" t="s">
         <v>435</v>
       </c>
@@ -5758,20 +5758,20 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="89" t="s">
+      <c r="A39" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="B39" s="87" t="s">
+      <c r="B39" s="86" t="s">
         <v>186</v>
       </c>
-      <c r="C39" s="85">
+      <c r="C39" s="84">
         <v>3</v>
       </c>
-      <c r="D39" s="90"/>
-      <c r="E39" s="87"/>
-      <c r="F39" s="87"/>
-      <c r="G39" s="86"/>
-      <c r="H39" s="88"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="85"/>
+      <c r="H39" s="87"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="63" t="s">
@@ -5783,27 +5783,27 @@
       <c r="C40" s="64">
         <v>3</v>
       </c>
-      <c r="D40" s="80"/>
+      <c r="D40" s="79"/>
       <c r="E40" s="26"/>
       <c r="F40" s="26"/>
       <c r="G40" s="65"/>
       <c r="H40" s="31"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="89" t="s">
+      <c r="A41" s="88" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="87" t="s">
+      <c r="B41" s="86" t="s">
         <v>188</v>
       </c>
-      <c r="C41" s="85">
+      <c r="C41" s="84">
         <v>3</v>
       </c>
-      <c r="D41" s="90"/>
-      <c r="E41" s="87"/>
-      <c r="F41" s="87"/>
-      <c r="G41" s="86"/>
-      <c r="H41" s="88"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="85"/>
+      <c r="H41" s="87"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="63" t="s">
@@ -5815,27 +5815,27 @@
       <c r="C42" s="64">
         <v>3</v>
       </c>
-      <c r="D42" s="80"/>
+      <c r="D42" s="79"/>
       <c r="E42" s="26"/>
       <c r="F42" s="26"/>
       <c r="G42" s="65"/>
       <c r="H42" s="31"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="89" t="s">
+      <c r="A43" s="88" t="s">
         <v>122</v>
       </c>
-      <c r="B43" s="87" t="s">
+      <c r="B43" s="86" t="s">
         <v>190</v>
       </c>
-      <c r="C43" s="85">
+      <c r="C43" s="84">
         <v>3</v>
       </c>
-      <c r="D43" s="90"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="86"/>
-      <c r="H43" s="88"/>
+      <c r="D43" s="89"/>
+      <c r="E43" s="90"/>
+      <c r="F43" s="90"/>
+      <c r="G43" s="85"/>
+      <c r="H43" s="87"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="63" t="s">
@@ -5847,27 +5847,27 @@
       <c r="C44" s="64">
         <v>3</v>
       </c>
-      <c r="D44" s="80"/>
+      <c r="D44" s="79"/>
       <c r="E44" s="66"/>
       <c r="F44" s="66"/>
       <c r="G44" s="65"/>
       <c r="H44" s="31"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="89" t="s">
+      <c r="A45" s="88" t="s">
         <v>124</v>
       </c>
-      <c r="B45" s="87" t="s">
+      <c r="B45" s="86" t="s">
         <v>192</v>
       </c>
-      <c r="C45" s="85">
+      <c r="C45" s="84">
         <v>3</v>
       </c>
-      <c r="D45" s="90"/>
-      <c r="E45" s="91"/>
-      <c r="F45" s="91"/>
-      <c r="G45" s="86"/>
-      <c r="H45" s="88"/>
+      <c r="D45" s="89"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="90"/>
+      <c r="G45" s="85"/>
+      <c r="H45" s="87"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="63" t="s">
@@ -5879,27 +5879,27 @@
       <c r="C46" s="64">
         <v>3</v>
       </c>
-      <c r="D46" s="80"/>
+      <c r="D46" s="79"/>
       <c r="E46" s="66"/>
       <c r="F46" s="66"/>
       <c r="G46" s="65"/>
       <c r="H46" s="31"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="89" t="s">
+      <c r="A47" s="88" t="s">
         <v>126</v>
       </c>
-      <c r="B47" s="87" t="s">
+      <c r="B47" s="86" t="s">
         <v>194</v>
       </c>
-      <c r="C47" s="85">
+      <c r="C47" s="84">
         <v>3</v>
       </c>
-      <c r="D47" s="90"/>
-      <c r="E47" s="91"/>
-      <c r="F47" s="91"/>
-      <c r="G47" s="86"/>
-      <c r="H47" s="88"/>
+      <c r="D47" s="89"/>
+      <c r="E47" s="90"/>
+      <c r="F47" s="90"/>
+      <c r="G47" s="85"/>
+      <c r="H47" s="87"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="63" t="s">
@@ -5911,27 +5911,27 @@
       <c r="C48" s="64">
         <v>3</v>
       </c>
-      <c r="D48" s="80"/>
+      <c r="D48" s="79"/>
       <c r="E48" s="66"/>
       <c r="F48" s="66"/>
       <c r="G48" s="65"/>
       <c r="H48" s="31"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="89" t="s">
+      <c r="A49" s="88" t="s">
         <v>128</v>
       </c>
-      <c r="B49" s="87" t="s">
+      <c r="B49" s="86" t="s">
         <v>196</v>
       </c>
-      <c r="C49" s="85">
+      <c r="C49" s="84">
         <v>3</v>
       </c>
-      <c r="D49" s="90"/>
-      <c r="E49" s="91"/>
-      <c r="F49" s="91"/>
-      <c r="G49" s="86"/>
-      <c r="H49" s="88"/>
+      <c r="D49" s="89"/>
+      <c r="E49" s="90"/>
+      <c r="F49" s="90"/>
+      <c r="G49" s="85"/>
+      <c r="H49" s="87"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="63" t="s">
@@ -5943,27 +5943,27 @@
       <c r="C50" s="64">
         <v>3</v>
       </c>
-      <c r="D50" s="80"/>
+      <c r="D50" s="79"/>
       <c r="E50" s="66"/>
       <c r="F50" s="66"/>
       <c r="G50" s="65"/>
       <c r="H50" s="31"/>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="89" t="s">
+      <c r="A51" s="88" t="s">
         <v>130</v>
       </c>
-      <c r="B51" s="87" t="s">
+      <c r="B51" s="86" t="s">
         <v>198</v>
       </c>
-      <c r="C51" s="85">
+      <c r="C51" s="84">
         <v>3</v>
       </c>
-      <c r="D51" s="90"/>
-      <c r="E51" s="91"/>
-      <c r="F51" s="91"/>
-      <c r="G51" s="86"/>
-      <c r="H51" s="88"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="90"/>
+      <c r="F51" s="90"/>
+      <c r="G51" s="85"/>
+      <c r="H51" s="87"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="63" t="s">
@@ -5975,7 +5975,7 @@
       <c r="C52" s="64">
         <v>3</v>
       </c>
-      <c r="D52" s="80"/>
+      <c r="D52" s="79"/>
       <c r="E52" s="66"/>
       <c r="F52" s="66"/>
       <c r="G52" s="65"/>
@@ -5984,20 +5984,20 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="89" t="s">
+      <c r="A53" s="88" t="s">
         <v>132</v>
       </c>
-      <c r="B53" s="87" t="s">
+      <c r="B53" s="86" t="s">
         <v>200</v>
       </c>
-      <c r="C53" s="85">
+      <c r="C53" s="84">
         <v>3</v>
       </c>
-      <c r="D53" s="90"/>
-      <c r="E53" s="91"/>
-      <c r="F53" s="91"/>
-      <c r="G53" s="86"/>
-      <c r="H53" s="88"/>
+      <c r="D53" s="89"/>
+      <c r="E53" s="90"/>
+      <c r="F53" s="90"/>
+      <c r="G53" s="85"/>
+      <c r="H53" s="87"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="63" t="s">
@@ -6009,27 +6009,27 @@
       <c r="C54" s="64">
         <v>3</v>
       </c>
-      <c r="D54" s="80"/>
+      <c r="D54" s="79"/>
       <c r="E54" s="66"/>
       <c r="F54" s="66"/>
       <c r="G54" s="65"/>
       <c r="H54" s="31"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="89" t="s">
+      <c r="A55" s="88" t="s">
         <v>134</v>
       </c>
-      <c r="B55" s="87" t="s">
+      <c r="B55" s="86" t="s">
         <v>202</v>
       </c>
-      <c r="C55" s="85">
+      <c r="C55" s="84">
         <v>3</v>
       </c>
-      <c r="D55" s="90"/>
-      <c r="E55" s="91"/>
-      <c r="F55" s="91"/>
-      <c r="G55" s="86"/>
-      <c r="H55" s="88"/>
+      <c r="D55" s="89"/>
+      <c r="E55" s="90"/>
+      <c r="F55" s="90"/>
+      <c r="G55" s="85"/>
+      <c r="H55" s="87"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="63" t="s">
@@ -6041,27 +6041,27 @@
       <c r="C56" s="64">
         <v>3</v>
       </c>
-      <c r="D56" s="80"/>
+      <c r="D56" s="79"/>
       <c r="E56" s="66"/>
       <c r="F56" s="66"/>
       <c r="G56" s="65"/>
       <c r="H56" s="31"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="89" t="s">
+      <c r="A57" s="88" t="s">
         <v>136</v>
       </c>
-      <c r="B57" s="87" t="s">
+      <c r="B57" s="86" t="s">
         <v>204</v>
       </c>
-      <c r="C57" s="85">
+      <c r="C57" s="84">
         <v>3</v>
       </c>
-      <c r="D57" s="90"/>
-      <c r="E57" s="91"/>
-      <c r="F57" s="91"/>
-      <c r="G57" s="86"/>
-      <c r="H57" s="88"/>
+      <c r="D57" s="89"/>
+      <c r="E57" s="90"/>
+      <c r="F57" s="90"/>
+      <c r="G57" s="85"/>
+      <c r="H57" s="87"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="63" t="s">
@@ -6073,7 +6073,7 @@
       <c r="C58" s="64">
         <v>6</v>
       </c>
-      <c r="D58" s="80"/>
+      <c r="D58" s="79"/>
       <c r="E58" s="66"/>
       <c r="F58" s="66"/>
       <c r="G58" s="65"/>
@@ -6082,25 +6082,25 @@
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="89" t="s">
+      <c r="A59" s="88" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="87" t="s">
+      <c r="B59" s="86" t="s">
         <v>206</v>
       </c>
-      <c r="C59" s="85">
+      <c r="C59" s="84">
         <v>6</v>
       </c>
-      <c r="D59" s="90"/>
-      <c r="E59" s="91"/>
-      <c r="F59" s="91"/>
-      <c r="G59" s="86"/>
-      <c r="H59" s="88" t="s">
+      <c r="D59" s="89"/>
+      <c r="E59" s="90"/>
+      <c r="F59" s="90"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="87" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="79" t="s">
+      <c r="A60" s="78" t="s">
         <v>139</v>
       </c>
       <c r="B60" s="26" t="s">
@@ -6109,7 +6109,7 @@
       <c r="C60" s="64">
         <v>1</v>
       </c>
-      <c r="D60" s="80"/>
+      <c r="D60" s="79"/>
       <c r="E60" s="66" t="s">
         <v>487</v>
       </c>
@@ -6124,26 +6124,26 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="24">
-      <c r="A61" s="89" t="s">
+      <c r="A61" s="88" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="87" t="s">
+      <c r="B61" s="86" t="s">
         <v>422</v>
       </c>
-      <c r="C61" s="85">
+      <c r="C61" s="84">
         <v>1</v>
       </c>
-      <c r="D61" s="90"/>
-      <c r="E61" s="87" t="s">
+      <c r="D61" s="89"/>
+      <c r="E61" s="86" t="s">
         <v>459</v>
       </c>
-      <c r="F61" s="87" t="s">
+      <c r="F61" s="86" t="s">
         <v>460</v>
       </c>
-      <c r="G61" s="86" t="s">
+      <c r="G61" s="85" t="s">
         <v>461</v>
       </c>
-      <c r="H61" s="88" t="s">
+      <c r="H61" s="87" t="s">
         <v>462</v>
       </c>
     </row>
@@ -6154,10 +6154,10 @@
       <c r="B62" s="26" t="s">
         <v>422</v>
       </c>
-      <c r="C62" s="81">
+      <c r="C62" s="80">
         <v>1</v>
       </c>
-      <c r="D62" s="82"/>
+      <c r="D62" s="81"/>
       <c r="E62" s="26" t="s">
         <v>418</v>
       </c>
@@ -6172,26 +6172,26 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="24">
-      <c r="A63" s="89" t="s">
+      <c r="A63" s="88" t="s">
         <v>142</v>
       </c>
-      <c r="B63" s="87" t="s">
+      <c r="B63" s="86" t="s">
         <v>408</v>
       </c>
-      <c r="C63" s="85">
+      <c r="C63" s="84">
         <v>1</v>
       </c>
-      <c r="D63" s="90"/>
-      <c r="E63" s="87" t="s">
+      <c r="D63" s="89"/>
+      <c r="E63" s="86" t="s">
         <v>409</v>
       </c>
-      <c r="F63" s="87" t="s">
+      <c r="F63" s="86" t="s">
         <v>410</v>
       </c>
-      <c r="G63" s="86" t="s">
+      <c r="G63" s="85" t="s">
         <v>411</v>
       </c>
-      <c r="H63" s="88" t="s">
+      <c r="H63" s="87" t="s">
         <v>618</v>
       </c>
     </row>
@@ -6205,33 +6205,33 @@
       <c r="C64" s="64">
         <v>1</v>
       </c>
-      <c r="D64" s="80"/>
+      <c r="D64" s="79"/>
       <c r="E64" s="26"/>
       <c r="F64" s="26"/>
       <c r="G64" s="65"/>
       <c r="H64" s="31"/>
     </row>
     <row r="65" spans="1:8" ht="45">
-      <c r="A65" s="89" t="s">
+      <c r="A65" s="88" t="s">
         <v>144</v>
       </c>
-      <c r="B65" s="87" t="s">
+      <c r="B65" s="86" t="s">
         <v>208</v>
       </c>
-      <c r="C65" s="85">
+      <c r="C65" s="84">
         <v>4</v>
       </c>
-      <c r="D65" s="90"/>
-      <c r="E65" s="87" t="s">
+      <c r="D65" s="89"/>
+      <c r="E65" s="86" t="s">
         <v>295</v>
       </c>
-      <c r="F65" s="87" t="s">
+      <c r="F65" s="86" t="s">
         <v>296</v>
       </c>
-      <c r="G65" s="86" t="s">
+      <c r="G65" s="85" t="s">
         <v>297</v>
       </c>
-      <c r="H65" s="88" t="s">
+      <c r="H65" s="87" t="s">
         <v>604</v>
       </c>
     </row>
@@ -6245,7 +6245,7 @@
       <c r="C66" s="64">
         <v>9</v>
       </c>
-      <c r="D66" s="80"/>
+      <c r="D66" s="79"/>
       <c r="E66" s="26" t="s">
         <v>465</v>
       </c>
@@ -6260,26 +6260,26 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="30">
-      <c r="A67" s="89" t="s">
+      <c r="A67" s="88" t="s">
         <v>146</v>
       </c>
-      <c r="B67" s="87" t="s">
+      <c r="B67" s="86" t="s">
         <v>209</v>
       </c>
-      <c r="C67" s="85">
+      <c r="C67" s="84">
         <v>5</v>
       </c>
-      <c r="D67" s="90"/>
-      <c r="E67" s="87" t="s">
+      <c r="D67" s="89"/>
+      <c r="E67" s="86" t="s">
         <v>468</v>
       </c>
-      <c r="F67" s="87" t="s">
+      <c r="F67" s="86" t="s">
         <v>469</v>
       </c>
-      <c r="G67" s="86" t="s">
+      <c r="G67" s="85" t="s">
         <v>470</v>
       </c>
-      <c r="H67" s="88" t="s">
+      <c r="H67" s="87" t="s">
         <v>463</v>
       </c>
     </row>
@@ -6293,7 +6293,7 @@
       <c r="C68" s="64">
         <v>5</v>
       </c>
-      <c r="D68" s="80"/>
+      <c r="D68" s="79"/>
       <c r="E68" s="26" t="s">
         <v>456</v>
       </c>
@@ -6308,26 +6308,26 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="30">
-      <c r="A69" s="89" t="s">
+      <c r="A69" s="88" t="s">
         <v>148</v>
       </c>
-      <c r="B69" s="87" t="s">
+      <c r="B69" s="86" t="s">
         <v>211</v>
       </c>
-      <c r="C69" s="85">
+      <c r="C69" s="84">
         <v>4</v>
       </c>
-      <c r="D69" s="90"/>
-      <c r="E69" s="87" t="s">
+      <c r="D69" s="89"/>
+      <c r="E69" s="86" t="s">
         <v>423</v>
       </c>
-      <c r="F69" s="87" t="s">
+      <c r="F69" s="86" t="s">
         <v>424</v>
       </c>
-      <c r="G69" s="86" t="s">
+      <c r="G69" s="85" t="s">
         <v>425</v>
       </c>
-      <c r="H69" s="88" t="s">
+      <c r="H69" s="87" t="s">
         <v>631</v>
       </c>
     </row>
@@ -6341,7 +6341,7 @@
       <c r="C70" s="64">
         <v>4</v>
       </c>
-      <c r="D70" s="80"/>
+      <c r="D70" s="79"/>
       <c r="E70" s="26" t="s">
         <v>426</v>
       </c>
@@ -6356,26 +6356,26 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="30">
-      <c r="A71" s="89" t="s">
+      <c r="A71" s="88" t="s">
         <v>150</v>
       </c>
-      <c r="B71" s="87" t="s">
+      <c r="B71" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="C71" s="85">
+      <c r="C71" s="84">
         <v>4</v>
       </c>
-      <c r="D71" s="90"/>
-      <c r="E71" s="87" t="s">
+      <c r="D71" s="89"/>
+      <c r="E71" s="86" t="s">
         <v>432</v>
       </c>
-      <c r="F71" s="87" t="s">
+      <c r="F71" s="86" t="s">
         <v>433</v>
       </c>
-      <c r="G71" s="86" t="s">
+      <c r="G71" s="85" t="s">
         <v>434</v>
       </c>
-      <c r="H71" s="88" t="s">
+      <c r="H71" s="87" t="s">
         <v>617</v>
       </c>
     </row>
@@ -6389,7 +6389,7 @@
       <c r="C72" s="64">
         <v>4</v>
       </c>
-      <c r="D72" s="80"/>
+      <c r="D72" s="79"/>
       <c r="E72" s="26" t="s">
         <v>429</v>
       </c>
@@ -6404,26 +6404,26 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="30">
-      <c r="A73" s="89" t="s">
+      <c r="A73" s="88" t="s">
         <v>152</v>
       </c>
-      <c r="B73" s="87" t="s">
+      <c r="B73" s="86" t="s">
         <v>228</v>
       </c>
-      <c r="C73" s="85">
+      <c r="C73" s="84">
         <v>12</v>
       </c>
-      <c r="D73" s="90"/>
-      <c r="E73" s="87" t="s">
+      <c r="D73" s="89"/>
+      <c r="E73" s="86" t="s">
         <v>588</v>
       </c>
-      <c r="F73" s="87" t="s">
+      <c r="F73" s="86" t="s">
         <v>589</v>
       </c>
-      <c r="G73" s="86" t="s">
+      <c r="G73" s="85" t="s">
         <v>441</v>
       </c>
-      <c r="H73" s="88" t="s">
+      <c r="H73" s="87" t="s">
         <v>590</v>
       </c>
     </row>
@@ -6437,7 +6437,7 @@
       <c r="C74" s="64" t="s">
         <v>294</v>
       </c>
-      <c r="D74" s="80"/>
+      <c r="D74" s="79"/>
       <c r="E74" s="26" t="s">
         <v>583</v>
       </c>
@@ -6452,26 +6452,26 @@
       </c>
     </row>
     <row r="75" spans="1:8" ht="30">
-      <c r="A75" s="89" t="s">
+      <c r="A75" s="88" t="s">
         <v>154</v>
       </c>
-      <c r="B75" s="87" t="s">
+      <c r="B75" s="86" t="s">
         <v>291</v>
       </c>
-      <c r="C75" s="85" t="s">
+      <c r="C75" s="84" t="s">
         <v>294</v>
       </c>
-      <c r="D75" s="90"/>
-      <c r="E75" s="91" t="s">
+      <c r="D75" s="89"/>
+      <c r="E75" s="90" t="s">
         <v>471</v>
       </c>
-      <c r="F75" s="91" t="s">
+      <c r="F75" s="90" t="s">
         <v>472</v>
       </c>
-      <c r="G75" s="86" t="s">
+      <c r="G75" s="85" t="s">
         <v>473</v>
       </c>
-      <c r="H75" s="88" t="s">
+      <c r="H75" s="87" t="s">
         <v>638</v>
       </c>
     </row>
@@ -6485,7 +6485,7 @@
       <c r="C76" s="64" t="s">
         <v>294</v>
       </c>
-      <c r="D76" s="80"/>
+      <c r="D76" s="79"/>
       <c r="E76" s="26" t="s">
         <v>474</v>
       </c>
@@ -6500,26 +6500,26 @@
       </c>
     </row>
     <row r="77" spans="1:8" ht="30">
-      <c r="A77" s="89" t="s">
+      <c r="A77" s="88" t="s">
         <v>156</v>
       </c>
-      <c r="B77" s="87" t="s">
+      <c r="B77" s="86" t="s">
         <v>293</v>
       </c>
-      <c r="C77" s="85" t="s">
+      <c r="C77" s="84" t="s">
         <v>294</v>
       </c>
-      <c r="D77" s="90"/>
-      <c r="E77" s="87" t="s">
+      <c r="D77" s="89"/>
+      <c r="E77" s="86" t="s">
         <v>479</v>
       </c>
-      <c r="F77" s="87" t="s">
+      <c r="F77" s="86" t="s">
         <v>480</v>
       </c>
-      <c r="G77" s="86" t="s">
+      <c r="G77" s="85" t="s">
         <v>481</v>
       </c>
-      <c r="H77" s="88" t="s">
+      <c r="H77" s="87" t="s">
         <v>636</v>
       </c>
     </row>
@@ -6533,7 +6533,7 @@
       <c r="C78" s="64" t="s">
         <v>360</v>
       </c>
-      <c r="D78" s="80"/>
+      <c r="D78" s="79"/>
       <c r="E78" s="26" t="s">
         <v>299</v>
       </c>
@@ -6548,26 +6548,26 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="30">
-      <c r="A79" s="89" t="s">
+      <c r="A79" s="88" t="s">
         <v>158</v>
       </c>
-      <c r="B79" s="87" t="s">
+      <c r="B79" s="86" t="s">
         <v>302</v>
       </c>
-      <c r="C79" s="85" t="s">
+      <c r="C79" s="84" t="s">
         <v>360</v>
       </c>
-      <c r="D79" s="90"/>
-      <c r="E79" s="87" t="s">
+      <c r="D79" s="89"/>
+      <c r="E79" s="86" t="s">
         <v>318</v>
       </c>
-      <c r="F79" s="87" t="s">
+      <c r="F79" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="G79" s="86" t="s">
+      <c r="G79" s="85" t="s">
         <v>320</v>
       </c>
-      <c r="H79" s="88" t="s">
+      <c r="H79" s="87" t="s">
         <v>605</v>
       </c>
     </row>
@@ -6581,7 +6581,7 @@
       <c r="C80" s="64" t="s">
         <v>360</v>
       </c>
-      <c r="D80" s="80"/>
+      <c r="D80" s="79"/>
       <c r="E80" s="26" t="s">
         <v>313</v>
       </c>
@@ -6596,26 +6596,26 @@
       </c>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="89" t="s">
+      <c r="A81" s="88" t="s">
         <v>160</v>
       </c>
-      <c r="B81" s="87" t="s">
+      <c r="B81" s="86" t="s">
         <v>304</v>
       </c>
-      <c r="C81" s="85" t="s">
+      <c r="C81" s="84" t="s">
         <v>360</v>
       </c>
-      <c r="D81" s="90"/>
-      <c r="E81" s="87" t="s">
+      <c r="D81" s="89"/>
+      <c r="E81" s="86" t="s">
         <v>309</v>
       </c>
-      <c r="F81" s="87" t="s">
+      <c r="F81" s="86" t="s">
         <v>310</v>
       </c>
-      <c r="G81" s="86" t="s">
+      <c r="G81" s="85" t="s">
         <v>311</v>
       </c>
-      <c r="H81" s="88" t="s">
+      <c r="H81" s="87" t="s">
         <v>626</v>
       </c>
     </row>
@@ -6629,7 +6629,7 @@
       <c r="C82" s="64" t="s">
         <v>360</v>
       </c>
-      <c r="D82" s="80"/>
+      <c r="D82" s="79"/>
       <c r="E82" s="26" t="s">
         <v>315</v>
       </c>
@@ -6644,26 +6644,26 @@
       </c>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" s="89" t="s">
+      <c r="A83" s="88" t="s">
         <v>162</v>
       </c>
-      <c r="B83" s="87" t="s">
+      <c r="B83" s="86" t="s">
         <v>306</v>
       </c>
-      <c r="C83" s="85" t="s">
+      <c r="C83" s="84" t="s">
         <v>361</v>
       </c>
-      <c r="D83" s="90"/>
-      <c r="E83" s="87" t="s">
+      <c r="D83" s="89"/>
+      <c r="E83" s="86" t="s">
         <v>307</v>
       </c>
-      <c r="F83" s="87" t="s">
+      <c r="F83" s="86" t="s">
         <v>308</v>
       </c>
-      <c r="G83" s="86" t="s">
+      <c r="G83" s="85" t="s">
         <v>312</v>
       </c>
-      <c r="H83" s="88" t="s">
+      <c r="H83" s="87" t="s">
         <v>623</v>
       </c>
     </row>
@@ -6677,7 +6677,7 @@
       <c r="C84" s="64" t="s">
         <v>360</v>
       </c>
-      <c r="D84" s="80"/>
+      <c r="D84" s="79"/>
       <c r="E84" s="26" t="s">
         <v>322</v>
       </c>
@@ -6692,26 +6692,26 @@
       </c>
     </row>
     <row r="85" spans="1:8">
-      <c r="A85" s="89" t="s">
+      <c r="A85" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="B85" s="87" t="s">
+      <c r="B85" s="86" t="s">
         <v>335</v>
       </c>
-      <c r="C85" s="85" t="s">
+      <c r="C85" s="84" t="s">
         <v>363</v>
       </c>
-      <c r="D85" s="90"/>
-      <c r="E85" s="87" t="s">
+      <c r="D85" s="89"/>
+      <c r="E85" s="86" t="s">
         <v>325</v>
       </c>
-      <c r="F85" s="87" t="s">
+      <c r="F85" s="86" t="s">
         <v>326</v>
       </c>
-      <c r="G85" s="86" t="s">
+      <c r="G85" s="85" t="s">
         <v>327</v>
       </c>
-      <c r="H85" s="88" t="s">
+      <c r="H85" s="87" t="s">
         <v>647</v>
       </c>
     </row>
@@ -6725,7 +6725,7 @@
       <c r="C86" s="64" t="s">
         <v>363</v>
       </c>
-      <c r="D86" s="80"/>
+      <c r="D86" s="79"/>
       <c r="E86" s="26" t="s">
         <v>328</v>
       </c>
@@ -6740,31 +6740,31 @@
       </c>
     </row>
     <row r="87" spans="1:8">
-      <c r="A87" s="89" t="s">
+      <c r="A87" s="88" t="s">
         <v>166</v>
       </c>
-      <c r="B87" s="87" t="s">
+      <c r="B87" s="86" t="s">
         <v>334</v>
       </c>
-      <c r="C87" s="85" t="s">
+      <c r="C87" s="84" t="s">
         <v>363</v>
       </c>
-      <c r="D87" s="90"/>
-      <c r="E87" s="87" t="s">
+      <c r="D87" s="89"/>
+      <c r="E87" s="86" t="s">
         <v>337</v>
       </c>
-      <c r="F87" s="87" t="s">
+      <c r="F87" s="86" t="s">
         <v>338</v>
       </c>
-      <c r="G87" s="86" t="s">
+      <c r="G87" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="H87" s="88" t="s">
+      <c r="H87" s="87" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="88" spans="1:8">
-      <c r="A88" s="79" t="s">
+      <c r="A88" s="78" t="s">
         <v>167</v>
       </c>
       <c r="B88" s="26" t="s">
@@ -6773,7 +6773,7 @@
       <c r="C88" s="64" t="s">
         <v>362</v>
       </c>
-      <c r="D88" s="80"/>
+      <c r="D88" s="79"/>
       <c r="E88" s="26" t="s">
         <v>340</v>
       </c>
@@ -6788,26 +6788,26 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="24">
-      <c r="A89" s="89" t="s">
+      <c r="A89" s="88" t="s">
         <v>168</v>
       </c>
-      <c r="B89" s="87" t="s">
+      <c r="B89" s="86" t="s">
         <v>343</v>
       </c>
-      <c r="C89" s="85" t="s">
+      <c r="C89" s="84" t="s">
         <v>294</v>
       </c>
-      <c r="D89" s="90"/>
-      <c r="E89" s="87" t="s">
+      <c r="D89" s="89"/>
+      <c r="E89" s="86" t="s">
         <v>344</v>
       </c>
-      <c r="F89" s="87" t="s">
+      <c r="F89" s="86" t="s">
         <v>452</v>
       </c>
-      <c r="G89" s="86" t="s">
+      <c r="G89" s="85" t="s">
         <v>345</v>
       </c>
-      <c r="H89" s="88" t="s">
+      <c r="H89" s="87" t="s">
         <v>625</v>
       </c>
     </row>
@@ -6821,7 +6821,7 @@
       <c r="C90" s="64" t="s">
         <v>362</v>
       </c>
-      <c r="D90" s="80"/>
+      <c r="D90" s="79"/>
       <c r="E90" s="26" t="s">
         <v>355</v>
       </c>
@@ -6836,26 +6836,26 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="30">
-      <c r="A91" s="89" t="s">
+      <c r="A91" s="88" t="s">
         <v>170</v>
       </c>
-      <c r="B91" s="87" t="s">
+      <c r="B91" s="86" t="s">
         <v>365</v>
       </c>
-      <c r="C91" s="85" t="s">
+      <c r="C91" s="84" t="s">
         <v>360</v>
       </c>
-      <c r="D91" s="90"/>
-      <c r="E91" s="87" t="s">
+      <c r="D91" s="89"/>
+      <c r="E91" s="86" t="s">
         <v>366</v>
       </c>
-      <c r="F91" s="87" t="s">
+      <c r="F91" s="86" t="s">
         <v>367</v>
       </c>
-      <c r="G91" s="86" t="s">
+      <c r="G91" s="85" t="s">
         <v>368</v>
       </c>
-      <c r="H91" s="88" t="s">
+      <c r="H91" s="87" t="s">
         <v>613</v>
       </c>
     </row>
@@ -6869,7 +6869,7 @@
       <c r="C92" s="64" t="s">
         <v>362</v>
       </c>
-      <c r="D92" s="80"/>
+      <c r="D92" s="79"/>
       <c r="E92" s="26" t="s">
         <v>380</v>
       </c>
@@ -6884,26 +6884,26 @@
       </c>
     </row>
     <row r="93" spans="1:8">
-      <c r="A93" s="89" t="s">
+      <c r="A93" s="88" t="s">
         <v>172</v>
       </c>
-      <c r="B93" s="87" t="s">
+      <c r="B93" s="86" t="s">
         <v>383</v>
       </c>
-      <c r="C93" s="85" t="s">
+      <c r="C93" s="84" t="s">
         <v>363</v>
       </c>
-      <c r="D93" s="90"/>
-      <c r="E93" s="87" t="s">
+      <c r="D93" s="89"/>
+      <c r="E93" s="86" t="s">
         <v>384</v>
       </c>
-      <c r="F93" s="87" t="s">
+      <c r="F93" s="86" t="s">
         <v>385</v>
       </c>
-      <c r="G93" s="86" t="s">
+      <c r="G93" s="85" t="s">
         <v>386</v>
       </c>
-      <c r="H93" s="88" t="s">
+      <c r="H93" s="87" t="s">
         <v>600</v>
       </c>
     </row>
@@ -6917,7 +6917,7 @@
       <c r="C94" s="64" t="s">
         <v>360</v>
       </c>
-      <c r="D94" s="80"/>
+      <c r="D94" s="79"/>
       <c r="E94" s="26" t="s">
         <v>387</v>
       </c>
@@ -6932,26 +6932,26 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="30">
-      <c r="A95" s="89" t="s">
+      <c r="A95" s="88" t="s">
         <v>174</v>
       </c>
-      <c r="B95" s="87" t="s">
+      <c r="B95" s="86" t="s">
         <v>406</v>
       </c>
-      <c r="C95" s="85" t="s">
+      <c r="C95" s="84" t="s">
         <v>363</v>
       </c>
-      <c r="D95" s="90"/>
-      <c r="E95" s="87" t="s">
+      <c r="D95" s="89"/>
+      <c r="E95" s="86" t="s">
         <v>404</v>
       </c>
-      <c r="F95" s="87" t="s">
+      <c r="F95" s="86" t="s">
         <v>407</v>
       </c>
-      <c r="G95" s="86">
+      <c r="G95" s="85">
         <v>1024</v>
       </c>
-      <c r="H95" s="88" t="s">
+      <c r="H95" s="87" t="s">
         <v>612</v>
       </c>
     </row>
@@ -6965,7 +6965,7 @@
       <c r="C96" s="64" t="s">
         <v>421</v>
       </c>
-      <c r="D96" s="80"/>
+      <c r="D96" s="79"/>
       <c r="E96" s="26" t="s">
         <v>415</v>
       </c>
@@ -6980,26 +6980,26 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="30">
-      <c r="A97" s="89" t="s">
+      <c r="A97" s="88" t="s">
         <v>176</v>
       </c>
-      <c r="B97" s="87" t="s">
+      <c r="B97" s="86" t="s">
         <v>438</v>
       </c>
-      <c r="C97" s="85" t="s">
+      <c r="C97" s="84" t="s">
         <v>360</v>
       </c>
-      <c r="D97" s="90"/>
-      <c r="E97" s="87" t="s">
+      <c r="D97" s="89"/>
+      <c r="E97" s="86" t="s">
         <v>439</v>
       </c>
-      <c r="F97" s="87" t="s">
+      <c r="F97" s="86" t="s">
         <v>440</v>
       </c>
-      <c r="G97" s="86" t="s">
+      <c r="G97" s="85" t="s">
         <v>441</v>
       </c>
-      <c r="H97" s="88" t="s">
+      <c r="H97" s="87" t="s">
         <v>628</v>
       </c>
     </row>
@@ -7013,7 +7013,7 @@
       <c r="C98" s="64" t="s">
         <v>649</v>
       </c>
-      <c r="D98" s="80"/>
+      <c r="D98" s="79"/>
       <c r="E98" s="26" t="s">
         <v>586</v>
       </c>
@@ -7028,26 +7028,26 @@
       </c>
     </row>
     <row r="99" spans="1:8">
-      <c r="A99" s="89" t="s">
+      <c r="A99" s="88" t="s">
         <v>178</v>
       </c>
-      <c r="B99" s="87" t="s">
+      <c r="B99" s="86" t="s">
         <v>448</v>
       </c>
-      <c r="C99" s="85" t="s">
+      <c r="C99" s="84" t="s">
         <v>649</v>
       </c>
-      <c r="D99" s="90"/>
-      <c r="E99" s="87" t="s">
+      <c r="D99" s="89"/>
+      <c r="E99" s="86" t="s">
         <v>445</v>
       </c>
-      <c r="F99" s="87" t="s">
+      <c r="F99" s="86" t="s">
         <v>446</v>
       </c>
-      <c r="G99" s="86" t="s">
+      <c r="G99" s="85" t="s">
         <v>447</v>
       </c>
-      <c r="H99" s="88" t="s">
+      <c r="H99" s="87" t="s">
         <v>443</v>
       </c>
     </row>
@@ -7061,7 +7061,7 @@
       <c r="C100" s="64" t="s">
         <v>649</v>
       </c>
-      <c r="D100" s="80"/>
+      <c r="D100" s="79"/>
       <c r="E100" s="26" t="s">
         <v>449</v>
       </c>
@@ -7076,26 +7076,26 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="30">
-      <c r="A101" s="89" t="s">
+      <c r="A101" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="B101" s="87" t="s">
+      <c r="B101" s="86" t="s">
         <v>306</v>
       </c>
-      <c r="C101" s="85" t="s">
+      <c r="C101" s="84" t="s">
         <v>360</v>
       </c>
-      <c r="D101" s="90"/>
-      <c r="E101" s="87" t="s">
+      <c r="D101" s="89"/>
+      <c r="E101" s="86" t="s">
         <v>490</v>
       </c>
-      <c r="F101" s="87" t="s">
+      <c r="F101" s="86" t="s">
         <v>491</v>
       </c>
-      <c r="G101" s="86" t="s">
+      <c r="G101" s="85" t="s">
         <v>492</v>
       </c>
-      <c r="H101" s="88" t="s">
+      <c r="H101" s="87" t="s">
         <v>643</v>
       </c>
     </row>
@@ -7109,7 +7109,7 @@
       <c r="C102" s="64" t="s">
         <v>363</v>
       </c>
-      <c r="D102" s="80"/>
+      <c r="D102" s="79"/>
       <c r="E102" s="66" t="s">
         <v>512</v>
       </c>
@@ -7124,26 +7124,26 @@
       </c>
     </row>
     <row r="103" spans="1:8">
-      <c r="A103" s="89" t="s">
+      <c r="A103" s="88" t="s">
         <v>182</v>
       </c>
-      <c r="B103" s="87" t="s">
+      <c r="B103" s="86" t="s">
         <v>537</v>
       </c>
-      <c r="C103" s="85" t="s">
+      <c r="C103" s="84" t="s">
         <v>648</v>
       </c>
-      <c r="D103" s="90"/>
-      <c r="E103" s="91" t="s">
+      <c r="D103" s="89"/>
+      <c r="E103" s="90" t="s">
         <v>538</v>
       </c>
-      <c r="F103" s="91" t="s">
+      <c r="F103" s="90" t="s">
         <v>539</v>
       </c>
-      <c r="G103" s="86" t="s">
+      <c r="G103" s="85" t="s">
         <v>540</v>
       </c>
-      <c r="H103" s="88" t="s">
+      <c r="H103" s="87" t="s">
         <v>541</v>
       </c>
     </row>
@@ -7157,7 +7157,7 @@
       <c r="C104" s="64" t="s">
         <v>360</v>
       </c>
-      <c r="D104" s="80"/>
+      <c r="D104" s="79"/>
       <c r="E104" s="66" t="s">
         <v>570</v>
       </c>
@@ -7172,26 +7172,26 @@
       </c>
     </row>
     <row r="105" spans="1:8">
-      <c r="A105" s="89" t="s">
+      <c r="A105" s="88" t="s">
         <v>563</v>
       </c>
-      <c r="B105" s="87" t="s">
+      <c r="B105" s="86" t="s">
         <v>579</v>
       </c>
-      <c r="C105" s="85" t="s">
+      <c r="C105" s="84" t="s">
         <v>360</v>
       </c>
-      <c r="D105" s="90"/>
-      <c r="E105" s="91" t="s">
+      <c r="D105" s="89"/>
+      <c r="E105" s="90" t="s">
         <v>580</v>
       </c>
-      <c r="F105" s="91" t="s">
+      <c r="F105" s="90" t="s">
         <v>581</v>
       </c>
-      <c r="G105" s="86" t="s">
+      <c r="G105" s="85" t="s">
         <v>577</v>
       </c>
-      <c r="H105" s="88" t="s">
+      <c r="H105" s="87" t="s">
         <v>644</v>
       </c>
     </row>
@@ -7205,7 +7205,7 @@
       <c r="C106" s="64" t="s">
         <v>360</v>
       </c>
-      <c r="D106" s="80"/>
+      <c r="D106" s="79"/>
       <c r="E106" s="66" t="s">
         <v>313</v>
       </c>
@@ -7220,16 +7220,16 @@
       </c>
     </row>
     <row r="107" spans="1:8">
-      <c r="A107" s="89" t="s">
+      <c r="A107" s="88" t="s">
         <v>565</v>
       </c>
-      <c r="B107" s="87"/>
-      <c r="C107" s="85"/>
-      <c r="D107" s="90"/>
-      <c r="E107" s="91"/>
-      <c r="F107" s="91"/>
-      <c r="G107" s="86"/>
-      <c r="H107" s="88"/>
+      <c r="B107" s="86"/>
+      <c r="C107" s="84"/>
+      <c r="D107" s="89"/>
+      <c r="E107" s="90"/>
+      <c r="F107" s="90"/>
+      <c r="G107" s="85"/>
+      <c r="H107" s="87"/>
     </row>
     <row r="108" spans="1:8">
       <c r="A108" s="63" t="s">
@@ -7237,34 +7237,34 @@
       </c>
       <c r="B108" s="26"/>
       <c r="C108" s="64"/>
-      <c r="D108" s="80"/>
+      <c r="D108" s="79"/>
       <c r="E108" s="66"/>
       <c r="F108" s="66"/>
       <c r="G108" s="65"/>
       <c r="H108" s="31"/>
     </row>
     <row r="109" spans="1:8">
-      <c r="A109" s="89" t="s">
+      <c r="A109" s="88" t="s">
         <v>567</v>
       </c>
-      <c r="B109" s="87"/>
-      <c r="C109" s="85"/>
-      <c r="D109" s="90"/>
-      <c r="E109" s="91"/>
-      <c r="F109" s="91"/>
-      <c r="G109" s="86"/>
-      <c r="H109" s="88"/>
+      <c r="B109" s="86"/>
+      <c r="C109" s="84"/>
+      <c r="D109" s="89"/>
+      <c r="E109" s="90"/>
+      <c r="F109" s="90"/>
+      <c r="G109" s="85"/>
+      <c r="H109" s="87"/>
     </row>
     <row r="110" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A110" s="75" t="s">
+      <c r="A110" s="74" t="s">
         <v>568</v>
       </c>
-      <c r="B110" s="76"/>
-      <c r="C110" s="77"/>
-      <c r="D110" s="93"/>
-      <c r="E110" s="94"/>
-      <c r="F110" s="94"/>
-      <c r="G110" s="78"/>
+      <c r="B110" s="75"/>
+      <c r="C110" s="76"/>
+      <c r="D110" s="92"/>
+      <c r="E110" s="93"/>
+      <c r="F110" s="93"/>
+      <c r="G110" s="77"/>
       <c r="H110" s="32"/>
     </row>
     <row r="111" spans="1:8">
@@ -9104,7 +9104,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1"/>
@@ -9144,34 +9144,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.9" customHeight="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="115" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="99"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="118" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="101"/>
+      <c r="B2" s="119"/>
       <c r="C2" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="104" t="s">
+      <c r="D2" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="103"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="121"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="K3" t="s">
@@ -9179,17 +9179,17 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="125" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="108"/>
-      <c r="C4" s="108"/>
-      <c r="D4" s="108"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="108"/>
-      <c r="G4" s="108"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="109"/>
+      <c r="B4" s="126"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="126"/>
+      <c r="I4" s="127"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="19" t="s">
@@ -9336,17 +9336,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="108" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="111"/>
-      <c r="C15" s="111"/>
-      <c r="D15" s="111"/>
-      <c r="E15" s="111"/>
-      <c r="F15" s="111"/>
-      <c r="G15" s="111"/>
-      <c r="H15" s="111"/>
-      <c r="I15" s="112"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="110"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="6" t="s">
@@ -9361,15 +9361,15 @@
       <c r="D16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="115" t="s">
+      <c r="E16" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="120"/>
-      <c r="G16" s="115" t="s">
+      <c r="F16" s="114"/>
+      <c r="G16" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="116"/>
-      <c r="I16" s="117"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="113"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="7">
@@ -9378,11 +9378,11 @@
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
-      <c r="E17" s="113"/>
-      <c r="F17" s="114"/>
-      <c r="G17" s="113"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="119"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="104"/>
+      <c r="H17" s="105"/>
+      <c r="I17" s="106"/>
       <c r="K17" t="s">
         <v>56</v>
       </c>
@@ -9394,11 +9394,11 @@
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
-      <c r="E18" s="113"/>
-      <c r="F18" s="114"/>
-      <c r="G18" s="113"/>
-      <c r="H18" s="118"/>
-      <c r="I18" s="119"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="107"/>
+      <c r="G18" s="104"/>
+      <c r="H18" s="105"/>
+      <c r="I18" s="106"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="7">
@@ -9407,11 +9407,11 @@
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
-      <c r="E19" s="113"/>
-      <c r="F19" s="114"/>
-      <c r="G19" s="113"/>
-      <c r="H19" s="118"/>
-      <c r="I19" s="119"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="105"/>
+      <c r="I19" s="106"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="7">
@@ -9420,11 +9420,11 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
-      <c r="E20" s="113"/>
-      <c r="F20" s="114"/>
-      <c r="G20" s="113"/>
-      <c r="H20" s="118"/>
-      <c r="I20" s="119"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="104"/>
+      <c r="H20" s="105"/>
+      <c r="I20" s="106"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="7">
@@ -9433,11 +9433,11 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="114"/>
-      <c r="G21" s="113"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="119"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="105"/>
+      <c r="I21" s="106"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="7">
@@ -9446,11 +9446,11 @@
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="113"/>
-      <c r="F22" s="114"/>
-      <c r="G22" s="113"/>
-      <c r="H22" s="118"/>
-      <c r="I22" s="119"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="107"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="106"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="7">
@@ -9459,11 +9459,11 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="114"/>
-      <c r="G23" s="113"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="119"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="106"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="7">
@@ -9472,11 +9472,11 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="113"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="113"/>
-      <c r="H24" s="118"/>
-      <c r="I24" s="119"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="107"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="106"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="7">
@@ -9485,11 +9485,11 @@
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="121"/>
-      <c r="F25" s="122"/>
-      <c r="G25" s="121"/>
-      <c r="H25" s="123"/>
-      <c r="I25" s="124"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="97"/>
+      <c r="G25" s="96"/>
+      <c r="H25" s="98"/>
+      <c r="I25" s="99"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1">
       <c r="A26" s="8">
@@ -9498,23 +9498,19 @@
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="125"/>
-      <c r="F26" s="126"/>
-      <c r="G26" s="125"/>
-      <c r="H26" s="127"/>
-      <c r="I26" s="128"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="101"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="102"/>
+      <c r="I26" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="A4:I4"/>
     <mergeCell ref="A15:I15"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
@@ -9529,11 +9525,15 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="E24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9562,50 +9562,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.9" customHeight="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="115" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="99"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="118" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="101"/>
+      <c r="B2" s="119"/>
       <c r="C2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="104" t="s">
+      <c r="D2" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="102" t="s">
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="103"/>
+      <c r="I2" s="121"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:17" ht="15.75">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="125" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="108"/>
-      <c r="C4" s="108"/>
-      <c r="D4" s="108"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="108"/>
-      <c r="G4" s="108"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="109"/>
+      <c r="B4" s="126"/>
+      <c r="C4" s="126"/>
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="126"/>
+      <c r="I4" s="127"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="19" t="s">
@@ -9667,15 +9667,15 @@
       <c r="I6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="K6" s="135" t="s">
+      <c r="K6" s="128" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
+      <c r="L6" s="128"/>
+      <c r="M6" s="128"/>
+      <c r="N6" s="128"/>
+      <c r="O6" s="128"/>
+      <c r="P6" s="128"/>
+      <c r="Q6" s="128"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="9">
@@ -9705,15 +9705,15 @@
       <c r="I7" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="135" t="s">
+      <c r="K7" s="128" t="s">
         <v>105</v>
       </c>
-      <c r="L7" s="135"/>
-      <c r="M7" s="135"/>
-      <c r="N7" s="135"/>
-      <c r="O7" s="135"/>
-      <c r="P7" s="135"/>
-      <c r="Q7" s="135"/>
+      <c r="L7" s="128"/>
+      <c r="M7" s="128"/>
+      <c r="N7" s="128"/>
+      <c r="O7" s="128"/>
+      <c r="P7" s="128"/>
+      <c r="Q7" s="128"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="9">
@@ -9821,17 +9821,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="108" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="111"/>
-      <c r="C15" s="111"/>
-      <c r="D15" s="111"/>
-      <c r="E15" s="111"/>
-      <c r="F15" s="111"/>
-      <c r="G15" s="111"/>
-      <c r="H15" s="111"/>
-      <c r="I15" s="112"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="109"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="110"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="19" t="s">
@@ -9846,15 +9846,15 @@
       <c r="D16" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="129" t="s">
+      <c r="E16" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="129"/>
-      <c r="G16" s="129" t="s">
+      <c r="F16" s="133"/>
+      <c r="G16" s="133" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="129"/>
-      <c r="I16" s="130"/>
+      <c r="H16" s="133"/>
+      <c r="I16" s="134"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="7">
@@ -9869,15 +9869,15 @@
       <c r="D17" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="131" t="s">
+      <c r="E17" s="129" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="132"/>
-      <c r="G17" s="131" t="s">
+      <c r="F17" s="130"/>
+      <c r="G17" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="133"/>
-      <c r="I17" s="134"/>
+      <c r="H17" s="131"/>
+      <c r="I17" s="132"/>
     </row>
     <row r="18" spans="1:11" ht="23.25">
       <c r="A18" s="7">
@@ -9892,15 +9892,15 @@
       <c r="D18" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="131" t="s">
+      <c r="E18" s="129" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="132"/>
-      <c r="G18" s="131" t="s">
+      <c r="F18" s="130"/>
+      <c r="G18" s="129" t="s">
         <v>85</v>
       </c>
-      <c r="H18" s="133"/>
-      <c r="I18" s="134"/>
+      <c r="H18" s="131"/>
+      <c r="I18" s="132"/>
     </row>
     <row r="19" spans="1:11" ht="34.5">
       <c r="A19" s="7">
@@ -9915,15 +9915,15 @@
       <c r="D19" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="131" t="s">
+      <c r="E19" s="129" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="132"/>
-      <c r="G19" s="131" t="s">
+      <c r="F19" s="130"/>
+      <c r="G19" s="129" t="s">
         <v>92</v>
       </c>
-      <c r="H19" s="133"/>
-      <c r="I19" s="134"/>
+      <c r="H19" s="131"/>
+      <c r="I19" s="132"/>
       <c r="K19" t="s">
         <v>56</v>
       </c>
@@ -9935,11 +9935,11 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
-      <c r="E20" s="113"/>
-      <c r="F20" s="114"/>
-      <c r="G20" s="113"/>
-      <c r="H20" s="118"/>
-      <c r="I20" s="119"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="104"/>
+      <c r="H20" s="105"/>
+      <c r="I20" s="106"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="7">
@@ -9948,11 +9948,11 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="114"/>
-      <c r="G21" s="113"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="119"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="104"/>
+      <c r="H21" s="105"/>
+      <c r="I21" s="106"/>
       <c r="K21" t="s">
         <v>81</v>
       </c>
@@ -9964,11 +9964,11 @@
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="113"/>
-      <c r="F22" s="114"/>
-      <c r="G22" s="113"/>
-      <c r="H22" s="118"/>
-      <c r="I22" s="119"/>
+      <c r="E22" s="104"/>
+      <c r="F22" s="107"/>
+      <c r="G22" s="104"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="106"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="7">
@@ -9977,11 +9977,11 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="114"/>
-      <c r="G23" s="113"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="119"/>
+      <c r="E23" s="104"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="104"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="106"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="7">
@@ -9990,11 +9990,11 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="113"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="113"/>
-      <c r="H24" s="118"/>
-      <c r="I24" s="119"/>
+      <c r="E24" s="104"/>
+      <c r="F24" s="107"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="106"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="7">
@@ -10003,11 +10003,11 @@
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="121"/>
-      <c r="F25" s="122"/>
-      <c r="G25" s="121"/>
-      <c r="H25" s="123"/>
-      <c r="I25" s="124"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="97"/>
+      <c r="G25" s="96"/>
+      <c r="H25" s="98"/>
+      <c r="I25" s="99"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1">
       <c r="A26" s="8">
@@ -10016,14 +10016,28 @@
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="125"/>
-      <c r="F26" s="126"/>
-      <c r="G26" s="125"/>
-      <c r="H26" s="127"/>
-      <c r="I26" s="128"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="101"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="102"/>
+      <c r="I26" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="K6:Q6"/>
@@ -10040,20 +10054,6 @@
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G20:I20"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10081,11 +10081,11 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="136" t="s">
+      <c r="A5" s="135" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="136"/>
-      <c r="C5" s="136"/>
+      <c r="B5" s="135"/>
+      <c r="C5" s="135"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="21" t="s">
@@ -10168,10 +10168,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15.75">
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="136" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="137"/>
+      <c r="C2" s="136"/>
       <c r="O2" t="s">
         <v>283</v>
       </c>
@@ -10411,56 +10411,56 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="136" t="s">
         <v>216</v>
       </c>
-      <c r="B3" s="137"/>
-      <c r="C3" s="137"/>
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="136" t="s">
+      <c r="B4" s="135" t="s">
         <v>223</v>
       </c>
-      <c r="C4" s="136"/>
+      <c r="C4" s="135"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="138" t="s">
+      <c r="B5" s="137" t="s">
         <v>222</v>
       </c>
-      <c r="C5" s="138"/>
+      <c r="C5" s="137"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="138" t="s">
+      <c r="B6" s="137" t="s">
         <v>217</v>
       </c>
-      <c r="C6" s="138"/>
+      <c r="C6" s="137"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="138" t="s">
+      <c r="B7" s="137" t="s">
         <v>218</v>
       </c>
-      <c r="C7" s="138"/>
+      <c r="C7" s="137"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="138" t="s">
+      <c r="B8" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="C8" s="138"/>
+      <c r="C8" s="137"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -10493,11 +10493,11 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:10" ht="15.75">
-      <c r="B2" s="139" t="s">
+      <c r="B2" s="138" t="s">
         <v>226</v>
       </c>
-      <c r="C2" s="140"/>
-      <c r="D2" s="141"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="140"/>
       <c r="J2" t="s">
         <v>283</v>
       </c>

</xml_diff>

<commit_message>
chg: Update tgt list
</commit_message>
<xml_diff>
--- a/OPAR/WORKSPACE/OPAR_JOINT_TARGET_LIST.xlsx
+++ b/OPAR/WORKSPACE/OPAR_JOINT_TARGET_LIST.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="670">
   <si>
     <t>NAME</t>
   </si>
@@ -2005,6 +2005,66 @@
   </si>
   <si>
     <t>11</t>
+  </si>
+  <si>
+    <t>N36 31.300</t>
+  </si>
+  <si>
+    <t>E037 02.300</t>
+  </si>
+  <si>
+    <t>1614ft</t>
+  </si>
+  <si>
+    <t>N36 11.000</t>
+  </si>
+  <si>
+    <t>E037 13.500</t>
+  </si>
+  <si>
+    <t>1258ft</t>
+  </si>
+  <si>
+    <t>E037 35.000</t>
+  </si>
+  <si>
+    <t>1201ft</t>
+  </si>
+  <si>
+    <t>N36 06.000</t>
+  </si>
+  <si>
+    <t>E037 56.000</t>
+  </si>
+  <si>
+    <t>1155ft</t>
+  </si>
+  <si>
+    <t>N35 45.500</t>
+  </si>
+  <si>
+    <t>E038 34.000</t>
+  </si>
+  <si>
+    <t>1066ft</t>
+  </si>
+  <si>
+    <t>N35 44.000</t>
+  </si>
+  <si>
+    <t>E037 06.000</t>
+  </si>
+  <si>
+    <t>820ft</t>
+  </si>
+  <si>
+    <t>N35 58.000</t>
+  </si>
+  <si>
+    <t>E036 47.000</t>
+  </si>
+  <si>
+    <t>1020ft</t>
   </si>
 </sst>
 </file>
@@ -2933,6 +2993,81 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2957,99 +3092,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3067,9 +3130,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3109,7 +3169,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3154,7 +3214,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3204,7 +3264,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3249,7 +3309,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3299,7 +3359,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3344,7 +3404,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3394,7 +3454,7 @@
         <xdr:cNvPr id="4" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3447,7 +3507,7 @@
         <xdr:cNvPr id="3" name="TekstSylinder 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3539,7 +3599,7 @@
         <xdr:cNvPr id="2049" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000001080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3597,7 +3657,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3650,7 +3710,7 @@
         <xdr:cNvPr id="2049" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000001080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3703,7 +3763,7 @@
         <xdr:cNvPr id="4" name="TekstSylinder 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3801,7 +3861,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3854,7 +3914,7 @@
         <xdr:cNvPr id="4" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3907,7 +3967,7 @@
         <xdr:cNvPr id="5" name="TekstSylinder 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4001,7 +4061,7 @@
         <xdr:cNvPr id="5" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4054,7 +4114,7 @@
         <xdr:cNvPr id="6" name="TekstSylinder 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4149,7 +4209,7 @@
         <xdr:cNvPr id="4" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4207,7 +4267,7 @@
         <xdr:cNvPr id="3073" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000010C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000010C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4260,7 +4320,7 @@
         <xdr:cNvPr id="3074" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000020C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000020C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4313,7 +4373,7 @@
         <xdr:cNvPr id="3075" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000030C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000030C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4366,7 +4426,7 @@
         <xdr:cNvPr id="3076" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000040C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000040C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4419,7 +4479,7 @@
         <xdr:cNvPr id="3077" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000050C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000050C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4472,7 +4532,7 @@
         <xdr:cNvPr id="3078" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000060C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000060C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4525,7 +4585,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4851,8 +4911,8 @@
   <dimension ref="A1:H317"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4877,7 +4937,7 @@
       <c r="E1" s="95"/>
       <c r="F1" s="95"/>
       <c r="G1" s="95"/>
-      <c r="H1" s="141"/>
+      <c r="H1" s="96"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1">
       <c r="A2" s="46" t="s">
@@ -5768,9 +5828,15 @@
         <v>3</v>
       </c>
       <c r="D39" s="89"/>
-      <c r="E39" s="86"/>
-      <c r="F39" s="86"/>
-      <c r="G39" s="85"/>
+      <c r="E39" s="86" t="s">
+        <v>650</v>
+      </c>
+      <c r="F39" s="86" t="s">
+        <v>651</v>
+      </c>
+      <c r="G39" s="85" t="s">
+        <v>652</v>
+      </c>
       <c r="H39" s="87"/>
     </row>
     <row r="40" spans="1:8">
@@ -5784,9 +5850,15 @@
         <v>3</v>
       </c>
       <c r="D40" s="79"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="65"/>
+      <c r="E40" s="26" t="s">
+        <v>653</v>
+      </c>
+      <c r="F40" s="26" t="s">
+        <v>654</v>
+      </c>
+      <c r="G40" s="65" t="s">
+        <v>655</v>
+      </c>
       <c r="H40" s="31"/>
     </row>
     <row r="41" spans="1:8">
@@ -5800,9 +5872,15 @@
         <v>3</v>
       </c>
       <c r="D41" s="89"/>
-      <c r="E41" s="86"/>
-      <c r="F41" s="86"/>
-      <c r="G41" s="85"/>
+      <c r="E41" s="86" t="s">
+        <v>653</v>
+      </c>
+      <c r="F41" s="86" t="s">
+        <v>656</v>
+      </c>
+      <c r="G41" s="85" t="s">
+        <v>657</v>
+      </c>
       <c r="H41" s="87"/>
     </row>
     <row r="42" spans="1:8">
@@ -5816,9 +5894,15 @@
         <v>3</v>
       </c>
       <c r="D42" s="79"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="65"/>
+      <c r="E42" s="26" t="s">
+        <v>658</v>
+      </c>
+      <c r="F42" s="26" t="s">
+        <v>659</v>
+      </c>
+      <c r="G42" s="65" t="s">
+        <v>660</v>
+      </c>
       <c r="H42" s="31"/>
     </row>
     <row r="43" spans="1:8">
@@ -5832,9 +5916,15 @@
         <v>3</v>
       </c>
       <c r="D43" s="89"/>
-      <c r="E43" s="90"/>
-      <c r="F43" s="90"/>
-      <c r="G43" s="85"/>
+      <c r="E43" s="90" t="s">
+        <v>661</v>
+      </c>
+      <c r="F43" s="90" t="s">
+        <v>662</v>
+      </c>
+      <c r="G43" s="85" t="s">
+        <v>663</v>
+      </c>
       <c r="H43" s="87"/>
     </row>
     <row r="44" spans="1:8">
@@ -5848,9 +5938,15 @@
         <v>3</v>
       </c>
       <c r="D44" s="79"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="66"/>
-      <c r="G44" s="65"/>
+      <c r="E44" s="66" t="s">
+        <v>664</v>
+      </c>
+      <c r="F44" s="66" t="s">
+        <v>665</v>
+      </c>
+      <c r="G44" s="65" t="s">
+        <v>666</v>
+      </c>
       <c r="H44" s="31"/>
     </row>
     <row r="45" spans="1:8">
@@ -5864,9 +5960,15 @@
         <v>3</v>
       </c>
       <c r="D45" s="89"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="90"/>
-      <c r="G45" s="85"/>
+      <c r="E45" s="90" t="s">
+        <v>667</v>
+      </c>
+      <c r="F45" s="90" t="s">
+        <v>668</v>
+      </c>
+      <c r="G45" s="85" t="s">
+        <v>669</v>
+      </c>
       <c r="H45" s="87"/>
     </row>
     <row r="46" spans="1:8">
@@ -9144,34 +9246,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.9" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="117"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="99"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="119"/>
+      <c r="B2" s="101"/>
       <c r="C2" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="122" t="s">
+      <c r="D2" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="121"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="103"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="K3" t="s">
@@ -9179,17 +9281,17 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="126"/>
-      <c r="C4" s="126"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
-      <c r="H4" s="126"/>
-      <c r="I4" s="127"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="109"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="19" t="s">
@@ -9336,17 +9438,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="110" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="109"/>
-      <c r="C15" s="109"/>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="110"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="111"/>
+      <c r="D15" s="111"/>
+      <c r="E15" s="111"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="111"/>
+      <c r="H15" s="111"/>
+      <c r="I15" s="112"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="6" t="s">
@@ -9361,15 +9463,15 @@
       <c r="D16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="111" t="s">
+      <c r="E16" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="114"/>
-      <c r="G16" s="111" t="s">
+      <c r="F16" s="120"/>
+      <c r="G16" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="112"/>
-      <c r="I16" s="113"/>
+      <c r="H16" s="116"/>
+      <c r="I16" s="117"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="7">
@@ -9378,11 +9480,11 @@
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="107"/>
-      <c r="G17" s="104"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="106"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="114"/>
+      <c r="G17" s="113"/>
+      <c r="H17" s="118"/>
+      <c r="I17" s="119"/>
       <c r="K17" t="s">
         <v>56</v>
       </c>
@@ -9394,11 +9496,11 @@
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="107"/>
-      <c r="G18" s="104"/>
-      <c r="H18" s="105"/>
-      <c r="I18" s="106"/>
+      <c r="E18" s="113"/>
+      <c r="F18" s="114"/>
+      <c r="G18" s="113"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="119"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="7">
@@ -9407,11 +9509,11 @@
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
-      <c r="E19" s="104"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="104"/>
-      <c r="H19" s="105"/>
-      <c r="I19" s="106"/>
+      <c r="E19" s="113"/>
+      <c r="F19" s="114"/>
+      <c r="G19" s="113"/>
+      <c r="H19" s="118"/>
+      <c r="I19" s="119"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="7">
@@ -9420,11 +9522,11 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="104"/>
-      <c r="H20" s="105"/>
-      <c r="I20" s="106"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="114"/>
+      <c r="G20" s="113"/>
+      <c r="H20" s="118"/>
+      <c r="I20" s="119"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="7">
@@ -9433,11 +9535,11 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="104"/>
-      <c r="H21" s="105"/>
-      <c r="I21" s="106"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="114"/>
+      <c r="G21" s="113"/>
+      <c r="H21" s="118"/>
+      <c r="I21" s="119"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="7">
@@ -9446,11 +9548,11 @@
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="107"/>
-      <c r="G22" s="104"/>
-      <c r="H22" s="105"/>
-      <c r="I22" s="106"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="114"/>
+      <c r="G22" s="113"/>
+      <c r="H22" s="118"/>
+      <c r="I22" s="119"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="7">
@@ -9459,11 +9561,11 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="107"/>
-      <c r="G23" s="104"/>
-      <c r="H23" s="105"/>
-      <c r="I23" s="106"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="114"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="118"/>
+      <c r="I23" s="119"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="7">
@@ -9472,11 +9574,11 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="107"/>
-      <c r="G24" s="104"/>
-      <c r="H24" s="105"/>
-      <c r="I24" s="106"/>
+      <c r="E24" s="113"/>
+      <c r="F24" s="114"/>
+      <c r="G24" s="113"/>
+      <c r="H24" s="118"/>
+      <c r="I24" s="119"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="7">
@@ -9485,11 +9587,11 @@
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="97"/>
-      <c r="G25" s="96"/>
-      <c r="H25" s="98"/>
-      <c r="I25" s="99"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="121"/>
+      <c r="H25" s="123"/>
+      <c r="I25" s="124"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1">
       <c r="A26" s="8">
@@ -9498,19 +9600,23 @@
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="100"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="102"/>
-      <c r="I26" s="103"/>
+      <c r="E26" s="125"/>
+      <c r="F26" s="126"/>
+      <c r="G26" s="125"/>
+      <c r="H26" s="127"/>
+      <c r="I26" s="128"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="E24:F24"/>
     <mergeCell ref="A15:I15"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
@@ -9525,15 +9631,11 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9562,50 +9664,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.9" customHeight="1">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="97" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="117"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="99"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="100" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="119"/>
+      <c r="B2" s="101"/>
       <c r="C2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="122" t="s">
+      <c r="D2" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="120" t="s">
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="102" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="121"/>
+      <c r="I2" s="103"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:17" ht="15.75">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="107" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="126"/>
-      <c r="C4" s="126"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
-      <c r="H4" s="126"/>
-      <c r="I4" s="127"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="108"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="108"/>
+      <c r="G4" s="108"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="109"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="19" t="s">
@@ -9667,15 +9769,15 @@
       <c r="I6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="K6" s="128" t="s">
+      <c r="K6" s="135" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="128"/>
-      <c r="M6" s="128"/>
-      <c r="N6" s="128"/>
-      <c r="O6" s="128"/>
-      <c r="P6" s="128"/>
-      <c r="Q6" s="128"/>
+      <c r="L6" s="135"/>
+      <c r="M6" s="135"/>
+      <c r="N6" s="135"/>
+      <c r="O6" s="135"/>
+      <c r="P6" s="135"/>
+      <c r="Q6" s="135"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="9">
@@ -9705,15 +9807,15 @@
       <c r="I7" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="135" t="s">
         <v>105</v>
       </c>
-      <c r="L7" s="128"/>
-      <c r="M7" s="128"/>
-      <c r="N7" s="128"/>
-      <c r="O7" s="128"/>
-      <c r="P7" s="128"/>
-      <c r="Q7" s="128"/>
+      <c r="L7" s="135"/>
+      <c r="M7" s="135"/>
+      <c r="N7" s="135"/>
+      <c r="O7" s="135"/>
+      <c r="P7" s="135"/>
+      <c r="Q7" s="135"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="9">
@@ -9821,17 +9923,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="110" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="109"/>
-      <c r="C15" s="109"/>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="110"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="111"/>
+      <c r="D15" s="111"/>
+      <c r="E15" s="111"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="111"/>
+      <c r="H15" s="111"/>
+      <c r="I15" s="112"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="19" t="s">
@@ -9846,15 +9948,15 @@
       <c r="D16" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="133" t="s">
+      <c r="E16" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="133"/>
-      <c r="G16" s="133" t="s">
+      <c r="F16" s="129"/>
+      <c r="G16" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="133"/>
-      <c r="I16" s="134"/>
+      <c r="H16" s="129"/>
+      <c r="I16" s="130"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="7">
@@ -9869,15 +9971,15 @@
       <c r="D17" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="129" t="s">
+      <c r="E17" s="131" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="130"/>
-      <c r="G17" s="129" t="s">
+      <c r="F17" s="132"/>
+      <c r="G17" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="131"/>
-      <c r="I17" s="132"/>
+      <c r="H17" s="133"/>
+      <c r="I17" s="134"/>
     </row>
     <row r="18" spans="1:11" ht="23.25">
       <c r="A18" s="7">
@@ -9892,15 +9994,15 @@
       <c r="D18" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="129" t="s">
+      <c r="E18" s="131" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="130"/>
-      <c r="G18" s="129" t="s">
+      <c r="F18" s="132"/>
+      <c r="G18" s="131" t="s">
         <v>85</v>
       </c>
-      <c r="H18" s="131"/>
-      <c r="I18" s="132"/>
+      <c r="H18" s="133"/>
+      <c r="I18" s="134"/>
     </row>
     <row r="19" spans="1:11" ht="34.5">
       <c r="A19" s="7">
@@ -9915,15 +10017,15 @@
       <c r="D19" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="129" t="s">
+      <c r="E19" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="130"/>
-      <c r="G19" s="129" t="s">
+      <c r="F19" s="132"/>
+      <c r="G19" s="131" t="s">
         <v>92</v>
       </c>
-      <c r="H19" s="131"/>
-      <c r="I19" s="132"/>
+      <c r="H19" s="133"/>
+      <c r="I19" s="134"/>
       <c r="K19" t="s">
         <v>56</v>
       </c>
@@ -9935,11 +10037,11 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="104"/>
-      <c r="H20" s="105"/>
-      <c r="I20" s="106"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="114"/>
+      <c r="G20" s="113"/>
+      <c r="H20" s="118"/>
+      <c r="I20" s="119"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="7">
@@ -9948,11 +10050,11 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="104"/>
-      <c r="H21" s="105"/>
-      <c r="I21" s="106"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="114"/>
+      <c r="G21" s="113"/>
+      <c r="H21" s="118"/>
+      <c r="I21" s="119"/>
       <c r="K21" t="s">
         <v>81</v>
       </c>
@@ -9964,11 +10066,11 @@
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="107"/>
-      <c r="G22" s="104"/>
-      <c r="H22" s="105"/>
-      <c r="I22" s="106"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="114"/>
+      <c r="G22" s="113"/>
+      <c r="H22" s="118"/>
+      <c r="I22" s="119"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="7">
@@ -9977,11 +10079,11 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="107"/>
-      <c r="G23" s="104"/>
-      <c r="H23" s="105"/>
-      <c r="I23" s="106"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="114"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="118"/>
+      <c r="I23" s="119"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="7">
@@ -9990,11 +10092,11 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="107"/>
-      <c r="G24" s="104"/>
-      <c r="H24" s="105"/>
-      <c r="I24" s="106"/>
+      <c r="E24" s="113"/>
+      <c r="F24" s="114"/>
+      <c r="G24" s="113"/>
+      <c r="H24" s="118"/>
+      <c r="I24" s="119"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="7">
@@ -10003,11 +10105,11 @@
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="97"/>
-      <c r="G25" s="96"/>
-      <c r="H25" s="98"/>
-      <c r="I25" s="99"/>
+      <c r="E25" s="121"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="121"/>
+      <c r="H25" s="123"/>
+      <c r="I25" s="124"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1">
       <c r="A26" s="8">
@@ -10016,28 +10118,14 @@
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="100"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="102"/>
-      <c r="I26" s="103"/>
+      <c r="E26" s="125"/>
+      <c r="F26" s="126"/>
+      <c r="G26" s="125"/>
+      <c r="H26" s="127"/>
+      <c r="I26" s="128"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="K6:Q6"/>
@@ -10054,6 +10142,20 @@
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G20:I20"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10081,11 +10183,11 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="135" t="s">
+      <c r="A5" s="136" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="135"/>
-      <c r="C5" s="135"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="136"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="21" t="s">
@@ -10168,10 +10270,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="15.75">
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="137" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="136"/>
+      <c r="C2" s="137"/>
       <c r="O2" t="s">
         <v>283</v>
       </c>
@@ -10411,56 +10513,56 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="137" t="s">
         <v>216</v>
       </c>
-      <c r="B3" s="136"/>
-      <c r="C3" s="136"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="136" t="s">
         <v>223</v>
       </c>
-      <c r="C4" s="135"/>
+      <c r="C4" s="136"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="137" t="s">
+      <c r="B5" s="138" t="s">
         <v>222</v>
       </c>
-      <c r="C5" s="137"/>
+      <c r="C5" s="138"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="137" t="s">
+      <c r="B6" s="138" t="s">
         <v>217</v>
       </c>
-      <c r="C6" s="137"/>
+      <c r="C6" s="138"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="138" t="s">
         <v>218</v>
       </c>
-      <c r="C7" s="137"/>
+      <c r="C7" s="138"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="137" t="s">
+      <c r="B8" s="138" t="s">
         <v>224</v>
       </c>
-      <c r="C8" s="137"/>
+      <c r="C8" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -10493,11 +10595,11 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:10" ht="15.75">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="139" t="s">
         <v>226</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="141"/>
       <c r="J2" t="s">
         <v>283</v>
       </c>

</xml_diff>

<commit_message>
chg: Added OPAR INTREP 001 and 004
</commit_message>
<xml_diff>
--- a/OPAR/WORKSPACE/OPAR_JOINT_TARGET_LIST.xlsx
+++ b/OPAR/WORKSPACE/OPAR_JOINT_TARGET_LIST.xlsx
@@ -3079,6 +3079,63 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3118,61 +3175,19 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3180,21 +3195,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3252,7 +3252,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3297,7 +3297,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3347,7 +3347,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3392,7 +3392,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3442,7 +3442,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3487,7 +3487,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3537,7 +3537,7 @@
         <xdr:cNvPr id="4" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3590,7 +3590,7 @@
         <xdr:cNvPr id="3" name="TekstSylinder 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3682,7 +3682,7 @@
         <xdr:cNvPr id="2049" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000001080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3740,7 +3740,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3793,7 +3793,7 @@
         <xdr:cNvPr id="2049" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000001080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3846,7 +3846,7 @@
         <xdr:cNvPr id="4" name="TekstSylinder 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3944,7 +3944,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3997,7 +3997,7 @@
         <xdr:cNvPr id="4" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4050,7 +4050,7 @@
         <xdr:cNvPr id="5" name="TekstSylinder 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4144,7 +4144,7 @@
         <xdr:cNvPr id="5" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4197,7 +4197,7 @@
         <xdr:cNvPr id="6" name="TekstSylinder 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4292,7 +4292,7 @@
         <xdr:cNvPr id="4" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4350,7 +4350,7 @@
         <xdr:cNvPr id="3073" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000010C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000010C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4403,7 +4403,7 @@
         <xdr:cNvPr id="3074" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000020C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000020C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4456,7 +4456,7 @@
         <xdr:cNvPr id="3075" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000030C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000030C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4509,7 +4509,7 @@
         <xdr:cNvPr id="3076" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000040C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000040C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4562,7 +4562,7 @@
         <xdr:cNvPr id="3077" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000050C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000050C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4615,7 +4615,7 @@
         <xdr:cNvPr id="3078" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000060C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000060C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4668,7 +4668,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5007,7 +5007,7 @@
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" style="40" customWidth="1"/>
-    <col min="8" max="8" width="65.140625" customWidth="1"/>
+    <col min="8" max="8" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.9" customHeight="1" thickBot="1">
@@ -9647,34 +9647,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.9" customHeight="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="119" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="102"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="121"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="104"/>
+      <c r="B2" s="123"/>
       <c r="C2" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="106"/>
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="125"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="K3" t="s">
@@ -9682,17 +9682,17 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="129" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="111"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="112"/>
+      <c r="B4" s="130"/>
+      <c r="C4" s="130"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="131"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="19" t="s">
@@ -9839,17 +9839,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="113" t="s">
+      <c r="A15" s="112" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="114"/>
-      <c r="F15" s="114"/>
-      <c r="G15" s="114"/>
-      <c r="H15" s="114"/>
-      <c r="I15" s="115"/>
+      <c r="B15" s="113"/>
+      <c r="C15" s="113"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="114"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="6" t="s">
@@ -9864,15 +9864,15 @@
       <c r="D16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="118" t="s">
+      <c r="E16" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="123"/>
-      <c r="G16" s="118" t="s">
+      <c r="F16" s="118"/>
+      <c r="G16" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="119"/>
-      <c r="I16" s="120"/>
+      <c r="H16" s="116"/>
+      <c r="I16" s="117"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="7">
@@ -9881,11 +9881,11 @@
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
-      <c r="E17" s="116"/>
-      <c r="F17" s="117"/>
-      <c r="G17" s="116"/>
-      <c r="H17" s="121"/>
-      <c r="I17" s="122"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="111"/>
+      <c r="G17" s="108"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="110"/>
       <c r="K17" t="s">
         <v>56</v>
       </c>
@@ -9897,11 +9897,11 @@
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
-      <c r="E18" s="116"/>
-      <c r="F18" s="117"/>
-      <c r="G18" s="116"/>
-      <c r="H18" s="121"/>
-      <c r="I18" s="122"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="110"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="7">
@@ -9910,11 +9910,11 @@
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
-      <c r="E19" s="116"/>
-      <c r="F19" s="117"/>
-      <c r="G19" s="116"/>
-      <c r="H19" s="121"/>
-      <c r="I19" s="122"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="110"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="7">
@@ -9923,11 +9923,11 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
-      <c r="E20" s="116"/>
-      <c r="F20" s="117"/>
-      <c r="G20" s="116"/>
-      <c r="H20" s="121"/>
-      <c r="I20" s="122"/>
+      <c r="E20" s="108"/>
+      <c r="F20" s="111"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="110"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="7">
@@ -9936,11 +9936,11 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
-      <c r="E21" s="116"/>
-      <c r="F21" s="117"/>
-      <c r="G21" s="116"/>
-      <c r="H21" s="121"/>
-      <c r="I21" s="122"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="110"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="7">
@@ -9949,11 +9949,11 @@
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="116"/>
-      <c r="F22" s="117"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="121"/>
-      <c r="I22" s="122"/>
+      <c r="E22" s="108"/>
+      <c r="F22" s="111"/>
+      <c r="G22" s="108"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="110"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="7">
@@ -9962,11 +9962,11 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="116"/>
-      <c r="F23" s="117"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="121"/>
-      <c r="I23" s="122"/>
+      <c r="E23" s="108"/>
+      <c r="F23" s="111"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="110"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="7">
@@ -9975,11 +9975,11 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="116"/>
-      <c r="F24" s="117"/>
-      <c r="G24" s="116"/>
-      <c r="H24" s="121"/>
-      <c r="I24" s="122"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="111"/>
+      <c r="G24" s="108"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="110"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="7">
@@ -9988,11 +9988,11 @@
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="124"/>
-      <c r="F25" s="125"/>
-      <c r="G25" s="124"/>
-      <c r="H25" s="126"/>
-      <c r="I25" s="127"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="101"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="102"/>
+      <c r="I25" s="103"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1">
       <c r="A26" s="8">
@@ -10001,23 +10001,19 @@
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="128"/>
-      <c r="F26" s="129"/>
-      <c r="G26" s="128"/>
-      <c r="H26" s="130"/>
-      <c r="I26" s="131"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="105"/>
+      <c r="G26" s="104"/>
+      <c r="H26" s="106"/>
+      <c r="I26" s="107"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="A4:I4"/>
     <mergeCell ref="A15:I15"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
@@ -10032,11 +10028,15 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="E24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10065,50 +10065,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.9" customHeight="1">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="119" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="102"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="121"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="104"/>
+      <c r="B2" s="123"/>
       <c r="C2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="126" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="105" t="s">
+      <c r="E2" s="127"/>
+      <c r="F2" s="127"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="124" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="106"/>
+      <c r="I2" s="125"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:17" ht="15.75">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="129" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="111"/>
-      <c r="C4" s="111"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="112"/>
+      <c r="B4" s="130"/>
+      <c r="C4" s="130"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="131"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="19" t="s">
@@ -10170,15 +10170,15 @@
       <c r="I6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="K6" s="138" t="s">
+      <c r="K6" s="132" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="138"/>
-      <c r="M6" s="138"/>
-      <c r="N6" s="138"/>
-      <c r="O6" s="138"/>
-      <c r="P6" s="138"/>
-      <c r="Q6" s="138"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="132"/>
+      <c r="Q6" s="132"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="9">
@@ -10208,15 +10208,15 @@
       <c r="I7" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="138" t="s">
+      <c r="K7" s="132" t="s">
         <v>105</v>
       </c>
-      <c r="L7" s="138"/>
-      <c r="M7" s="138"/>
-      <c r="N7" s="138"/>
-      <c r="O7" s="138"/>
-      <c r="P7" s="138"/>
-      <c r="Q7" s="138"/>
+      <c r="L7" s="132"/>
+      <c r="M7" s="132"/>
+      <c r="N7" s="132"/>
+      <c r="O7" s="132"/>
+      <c r="P7" s="132"/>
+      <c r="Q7" s="132"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="9">
@@ -10324,17 +10324,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="113" t="s">
+      <c r="A15" s="112" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="114"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="114"/>
-      <c r="F15" s="114"/>
-      <c r="G15" s="114"/>
-      <c r="H15" s="114"/>
-      <c r="I15" s="115"/>
+      <c r="B15" s="113"/>
+      <c r="C15" s="113"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="114"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="19" t="s">
@@ -10349,15 +10349,15 @@
       <c r="D16" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="132" t="s">
+      <c r="E16" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="132"/>
-      <c r="G16" s="132" t="s">
+      <c r="F16" s="137"/>
+      <c r="G16" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="132"/>
-      <c r="I16" s="133"/>
+      <c r="H16" s="137"/>
+      <c r="I16" s="138"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="7">
@@ -10372,15 +10372,15 @@
       <c r="D17" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="134" t="s">
+      <c r="E17" s="133" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="135"/>
-      <c r="G17" s="134" t="s">
+      <c r="F17" s="134"/>
+      <c r="G17" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="136"/>
-      <c r="I17" s="137"/>
+      <c r="H17" s="135"/>
+      <c r="I17" s="136"/>
     </row>
     <row r="18" spans="1:11" ht="23.25">
       <c r="A18" s="7">
@@ -10395,15 +10395,15 @@
       <c r="D18" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="134" t="s">
+      <c r="E18" s="133" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="135"/>
-      <c r="G18" s="134" t="s">
+      <c r="F18" s="134"/>
+      <c r="G18" s="133" t="s">
         <v>85</v>
       </c>
-      <c r="H18" s="136"/>
-      <c r="I18" s="137"/>
+      <c r="H18" s="135"/>
+      <c r="I18" s="136"/>
     </row>
     <row r="19" spans="1:11" ht="34.5">
       <c r="A19" s="7">
@@ -10418,15 +10418,15 @@
       <c r="D19" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="134" t="s">
+      <c r="E19" s="133" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="135"/>
-      <c r="G19" s="134" t="s">
+      <c r="F19" s="134"/>
+      <c r="G19" s="133" t="s">
         <v>92</v>
       </c>
-      <c r="H19" s="136"/>
-      <c r="I19" s="137"/>
+      <c r="H19" s="135"/>
+      <c r="I19" s="136"/>
       <c r="K19" t="s">
         <v>56</v>
       </c>
@@ -10438,11 +10438,11 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
-      <c r="E20" s="116"/>
-      <c r="F20" s="117"/>
-      <c r="G20" s="116"/>
-      <c r="H20" s="121"/>
-      <c r="I20" s="122"/>
+      <c r="E20" s="108"/>
+      <c r="F20" s="111"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="110"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="7">
@@ -10451,11 +10451,11 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
-      <c r="E21" s="116"/>
-      <c r="F21" s="117"/>
-      <c r="G21" s="116"/>
-      <c r="H21" s="121"/>
-      <c r="I21" s="122"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="110"/>
       <c r="K21" t="s">
         <v>81</v>
       </c>
@@ -10467,11 +10467,11 @@
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="116"/>
-      <c r="F22" s="117"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="121"/>
-      <c r="I22" s="122"/>
+      <c r="E22" s="108"/>
+      <c r="F22" s="111"/>
+      <c r="G22" s="108"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="110"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="7">
@@ -10480,11 +10480,11 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="116"/>
-      <c r="F23" s="117"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="121"/>
-      <c r="I23" s="122"/>
+      <c r="E23" s="108"/>
+      <c r="F23" s="111"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="110"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="7">
@@ -10493,11 +10493,11 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="116"/>
-      <c r="F24" s="117"/>
-      <c r="G24" s="116"/>
-      <c r="H24" s="121"/>
-      <c r="I24" s="122"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="111"/>
+      <c r="G24" s="108"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="110"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="7">
@@ -10506,11 +10506,11 @@
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="124"/>
-      <c r="F25" s="125"/>
-      <c r="G25" s="124"/>
-      <c r="H25" s="126"/>
-      <c r="I25" s="127"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="101"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="102"/>
+      <c r="I25" s="103"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1">
       <c r="A26" s="8">
@@ -10519,14 +10519,28 @@
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="128"/>
-      <c r="F26" s="129"/>
-      <c r="G26" s="128"/>
-      <c r="H26" s="130"/>
-      <c r="I26" s="131"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="105"/>
+      <c r="G26" s="104"/>
+      <c r="H26" s="106"/>
+      <c r="I26" s="107"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="K6:Q6"/>
@@ -10543,20 +10557,6 @@
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G20:I20"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>